<commit_message>
!(T to 20T map Add uid colimns for technical area, num or denom, and dissagg dimensiions
</commit_message>
<xml_diff>
--- a/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
+++ b/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/COP-19-Target-Setting/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/site_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{21DC5B28-1E72-A240-AACE-B929018E4F6E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E550A91F-7C3B-294C-A162-B00AE18455B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35600" yWindow="620" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3780" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1365" uniqueCount="381">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1368" uniqueCount="384">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -1176,6 +1176,15 @@
   </si>
   <si>
     <t>Disagregation Type_fy20_cop</t>
+  </si>
+  <si>
+    <t>technical_area_uid</t>
+  </si>
+  <si>
+    <t>num_or_den_uid</t>
+  </si>
+  <si>
+    <t>disagg_type_uid</t>
   </si>
 </sst>
 </file>
@@ -2042,20 +2051,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O77"/>
+  <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="67.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.33203125" customWidth="1"/>
+    <col min="18" max="18" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>374</v>
       </c>
@@ -2075,28 +2087,37 @@
         <v>204</v>
       </c>
       <c r="H1" t="s">
+        <v>381</v>
+      </c>
+      <c r="I1" t="s">
         <v>205</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>382</v>
+      </c>
+      <c r="K1" t="s">
         <v>379</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>383</v>
+      </c>
+      <c r="M1" t="s">
         <v>207</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>208</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>209</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>378</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -2116,29 +2137,32 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q2" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2158,29 +2182,32 @@
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q3" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -2200,29 +2227,32 @@
       <c r="G4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q4" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -2242,29 +2272,32 @@
       <c r="G5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1"/>
+      <c r="M5" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="O5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q5" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2284,29 +2317,32 @@
       <c r="G6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="1"/>
+      <c r="M6" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q6" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -2326,29 +2362,32 @@
       <c r="G7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q7" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -2368,29 +2407,32 @@
       <c r="G8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="1" t="s">
+      <c r="O8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q8" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2410,29 +2452,32 @@
       <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" s="1" t="s">
+      <c r="O9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q9" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -2452,29 +2497,32 @@
       <c r="G10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M10" s="1" t="s">
+      <c r="O10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q10" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -2494,29 +2542,32 @@
       <c r="G11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" s="1" t="s">
+      <c r="O11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q11" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -2536,29 +2587,32 @@
       <c r="G12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="L12" s="1"/>
+      <c r="M12" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M12" s="1" t="s">
+      <c r="O12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q12" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -2578,29 +2632,32 @@
       <c r="G13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="L13" s="1"/>
+      <c r="M13" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M13" s="1" t="s">
+      <c r="O13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+      <c r="Q13" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -2620,29 +2677,32 @@
       <c r="G14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="L14" s="1"/>
+      <c r="M14" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="N14" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M14" s="1" t="s">
+      <c r="O14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+      <c r="Q14" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -2662,29 +2722,32 @@
       <c r="G15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="L15" s="1"/>
+      <c r="M15" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="N15" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M15" s="1" t="s">
+      <c r="O15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q15" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -2704,29 +2767,32 @@
       <c r="G16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="L16" s="1"/>
+      <c r="M16" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M16" s="1" t="s">
+      <c r="O16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q16" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -2746,29 +2812,32 @@
       <c r="G17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="L17" s="1"/>
+      <c r="M17" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M17" s="1" t="s">
+      <c r="O17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q17" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -2788,29 +2857,32 @@
       <c r="G18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H18" s="1"/>
       <c r="I18" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="L18" s="1"/>
+      <c r="M18" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M18" s="1" t="s">
+      <c r="O18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N18" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q18" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
@@ -2830,29 +2902,32 @@
       <c r="G19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="L19" s="1"/>
+      <c r="M19" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M19" s="1" t="s">
+      <c r="O19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q19" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -2872,29 +2947,32 @@
       <c r="G20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="L20" s="1"/>
+      <c r="M20" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M20" s="1" t="s">
+      <c r="O20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q20" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
@@ -2914,29 +2992,32 @@
       <c r="G21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="L21" s="1"/>
+      <c r="M21" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M21" s="1" t="s">
+      <c r="O21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q21" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
@@ -2956,29 +3037,32 @@
       <c r="G22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="L22" s="1"/>
+      <c r="M22" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M22" s="1" t="s">
+      <c r="O22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q22" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>59</v>
       </c>
@@ -2998,29 +3082,32 @@
       <c r="G23" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="L23" s="1"/>
+      <c r="M23" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M23" s="1" t="s">
+      <c r="O23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P23" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q23" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -3040,29 +3127,32 @@
       <c r="G24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="L24" s="1"/>
+      <c r="M24" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M24" s="1" t="s">
+      <c r="O24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P24" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N24" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q24" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
@@ -3082,29 +3172,32 @@
       <c r="G25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="L25" s="1"/>
+      <c r="M25" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="L25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M25" s="1" t="s">
+      <c r="O25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P25" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q25" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
@@ -3124,29 +3217,32 @@
       <c r="G26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="L26" s="1"/>
+      <c r="M26" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M26" s="1" t="s">
+      <c r="O26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P26" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N26" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q26" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
@@ -3166,29 +3262,32 @@
       <c r="G27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="L27" s="1"/>
+      <c r="M27" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M27" s="1" t="s">
+      <c r="O27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P27" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="N27" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q27" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>66</v>
       </c>
@@ -3208,29 +3307,32 @@
       <c r="G28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H28" s="1"/>
       <c r="I28" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="L28" s="1"/>
+      <c r="M28" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M28" s="1" t="s">
+      <c r="O28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P28" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N28" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q28" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
@@ -3250,29 +3352,32 @@
       <c r="G29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H29" s="1"/>
       <c r="I29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="L29" s="1"/>
+      <c r="M29" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M29" s="1" t="s">
+      <c r="O29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P29" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="N29" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q29" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>69</v>
       </c>
@@ -3292,29 +3397,32 @@
       <c r="G30" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="L30" s="1"/>
+      <c r="M30" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="N30" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M30" s="1" t="s">
+      <c r="O30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P30" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N30" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q30" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>71</v>
       </c>
@@ -3334,29 +3442,32 @@
       <c r="G31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="L31" s="1"/>
+      <c r="M31" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M31" s="1" t="s">
+      <c r="O31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="N31" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q31" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
@@ -3376,29 +3487,32 @@
       <c r="G32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H32" s="1"/>
       <c r="I32" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L32" s="1" t="s">
+      <c r="L32" s="1"/>
+      <c r="M32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O32" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="P32" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="N32" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q32" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>75</v>
       </c>
@@ -3418,29 +3532,32 @@
       <c r="G33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H33" s="1"/>
       <c r="I33" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L33" s="1" t="s">
+      <c r="L33" s="1"/>
+      <c r="M33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O33" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="P33" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="N33" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q33" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
@@ -3460,29 +3577,32 @@
       <c r="G34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1"/>
+      <c r="M34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N34" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>79</v>
       </c>
@@ -3502,29 +3622,32 @@
       <c r="G35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L35" s="1" t="s">
+      <c r="L35" s="1"/>
+      <c r="M35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O35" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="M35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
@@ -3544,29 +3667,32 @@
       <c r="G36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="L36" s="1"/>
       <c r="M36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
@@ -3586,29 +3712,32 @@
       <c r="G37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="L37" s="1"/>
+      <c r="M37" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>89</v>
       </c>
@@ -3628,29 +3757,32 @@
       <c r="G38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="L38" s="1"/>
+      <c r="M38" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="N38" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>91</v>
       </c>
@@ -3670,29 +3802,32 @@
       <c r="G39" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H39" s="1"/>
       <c r="I39" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1"/>
+      <c r="M39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N39" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M39" s="1" t="s">
+      <c r="O39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P39" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="N39" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q39" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>95</v>
       </c>
@@ -3712,29 +3847,32 @@
       <c r="G40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H40" s="1"/>
       <c r="I40" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1"/>
+      <c r="M40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N40" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M40" s="1" t="s">
+      <c r="O40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P40" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="N40" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q40" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
@@ -3754,29 +3892,32 @@
       <c r="G41" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H41" s="1"/>
       <c r="I41" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="L41" s="1"/>
+      <c r="M41" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="K41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="N41" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>101</v>
       </c>
@@ -3796,29 +3937,32 @@
       <c r="G42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H42" s="1"/>
       <c r="I42" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J42" s="7" t="s">
+      <c r="L42" s="1"/>
+      <c r="M42" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="K42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="N42" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>103</v>
       </c>
@@ -3838,29 +3982,32 @@
       <c r="G43" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H43" s="1"/>
+      <c r="I43" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="J43" s="1"/>
+      <c r="K43" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="L43" s="1"/>
+      <c r="M43" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="N43" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="L43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>106</v>
       </c>
@@ -3880,29 +4027,32 @@
       <c r="G44" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H44" s="1"/>
       <c r="I44" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="L44" s="1"/>
+      <c r="M44" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="L44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M44" s="7" t="s">
+      <c r="O44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P44" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="N44" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q44" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>109</v>
       </c>
@@ -3922,29 +4072,32 @@
       <c r="G45" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H45" s="1"/>
       <c r="I45" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="L45" s="1"/>
+      <c r="M45" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="N45" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="L45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M45" s="7" t="s">
+      <c r="O45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P45" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="N45" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q45" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>110</v>
       </c>
@@ -3964,29 +4117,32 @@
       <c r="G46" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H46" s="1"/>
       <c r="I46" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="L46" s="1"/>
+      <c r="M46" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="N46" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="L46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M46" s="7" t="s">
+      <c r="O46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P46" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="N46" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q46" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>111</v>
       </c>
@@ -4006,29 +4162,32 @@
       <c r="G47" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H47" s="1"/>
       <c r="I47" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="L47" s="1"/>
+      <c r="M47" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="N47" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M47" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="N47" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>113</v>
       </c>
@@ -4048,29 +4207,32 @@
       <c r="G48" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H48" s="1"/>
       <c r="I48" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="L48" s="1"/>
+      <c r="M48" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="N48" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N48" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>115</v>
       </c>
@@ -4090,29 +4252,32 @@
       <c r="G49" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H49" s="1"/>
       <c r="I49" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L49" s="1" t="s">
+      <c r="L49" s="1"/>
+      <c r="M49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O49" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="M49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N49" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q49" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>116</v>
       </c>
@@ -4132,29 +4297,32 @@
       <c r="G50" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H50" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="L50" s="1"/>
+      <c r="M50" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="N50" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M50" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="N50" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P50" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q50" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>118</v>
       </c>
@@ -4174,29 +4342,32 @@
       <c r="G51" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H51" s="1"/>
       <c r="I51" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L51" s="1" t="s">
+      <c r="L51" s="1"/>
+      <c r="M51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O51" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="M51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q51" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>119</v>
       </c>
@@ -4216,29 +4387,32 @@
       <c r="G52" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H52" s="1"/>
       <c r="I52" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J52" s="8" t="s">
+      <c r="L52" s="1"/>
+      <c r="M52" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K52" s="1" t="s">
+      <c r="N52" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>122</v>
       </c>
@@ -4258,29 +4432,32 @@
       <c r="G53" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H53" s="1"/>
       <c r="I53" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J53" s="8" t="s">
+      <c r="L53" s="1"/>
+      <c r="M53" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="N53" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N53" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q53" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>123</v>
       </c>
@@ -4300,29 +4477,32 @@
       <c r="G54" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="H54" s="1"/>
+      <c r="I54" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="J54" s="1"/>
+      <c r="K54" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J54" s="8" t="s">
+      <c r="L54" s="1"/>
+      <c r="M54" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="N54" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N54" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>127</v>
       </c>
@@ -4342,29 +4522,32 @@
       <c r="G55" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="H55" s="1"/>
+      <c r="I55" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="J55" s="1"/>
+      <c r="K55" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J55" s="8" t="s">
+      <c r="L55" s="1"/>
+      <c r="M55" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="N55" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N55" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q55" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>129</v>
       </c>
@@ -4384,29 +4567,32 @@
       <c r="G56" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="H56" s="1"/>
+      <c r="I56" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="J56" s="1"/>
+      <c r="K56" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J56" s="8" t="s">
+      <c r="L56" s="1"/>
+      <c r="M56" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K56" s="1" t="s">
+      <c r="N56" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N56" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>131</v>
       </c>
@@ -4426,29 +4612,32 @@
       <c r="G57" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="H57" s="1"/>
+      <c r="I57" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I57" s="1" t="s">
+      <c r="J57" s="1"/>
+      <c r="K57" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J57" s="8" t="s">
+      <c r="L57" s="1"/>
+      <c r="M57" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K57" s="1" t="s">
+      <c r="N57" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N57" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>133</v>
       </c>
@@ -4468,29 +4657,32 @@
       <c r="G58" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H58" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H58" s="1"/>
       <c r="I58" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J58" s="8" t="s">
+      <c r="L58" s="1"/>
+      <c r="M58" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="N58" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N58" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>134</v>
       </c>
@@ -4510,29 +4702,32 @@
       <c r="G59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H59" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H59" s="1"/>
       <c r="I59" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J59" s="8" t="s">
+      <c r="L59" s="1"/>
+      <c r="M59" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K59" s="1" t="s">
+      <c r="N59" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L59" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M59" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N59" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>135</v>
       </c>
@@ -4552,29 +4747,32 @@
       <c r="G60" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H60" s="1"/>
       <c r="I60" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J60" s="8" t="s">
+      <c r="L60" s="1"/>
+      <c r="M60" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="N60" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L60" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M60" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N60" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>136</v>
       </c>
@@ -4594,29 +4792,32 @@
       <c r="G61" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H61" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H61" s="1"/>
       <c r="I61" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J61" s="8" t="s">
+      <c r="L61" s="1"/>
+      <c r="M61" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K61" s="1" t="s">
+      <c r="N61" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N61" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q61" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>137</v>
       </c>
@@ -4636,29 +4837,32 @@
       <c r="G62" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="H62" s="1"/>
+      <c r="I62" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I62" s="1" t="s">
+      <c r="J62" s="1"/>
+      <c r="K62" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="J62" s="8" t="s">
+      <c r="L62" s="1"/>
+      <c r="M62" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K62" s="1" t="s">
+      <c r="N62" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L62" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N62" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q62" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>139</v>
       </c>
@@ -4678,29 +4882,32 @@
       <c r="G63" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H63" s="1"/>
       <c r="I63" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="J63" s="8" t="s">
+      <c r="L63" s="1"/>
+      <c r="M63" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K63" s="1" t="s">
+      <c r="N63" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L63" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M63" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N63" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q63" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>141</v>
       </c>
@@ -4720,29 +4927,32 @@
       <c r="G64" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H64" s="1"/>
       <c r="I64" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="J64" s="8" t="s">
+      <c r="L64" s="1"/>
+      <c r="M64" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K64" s="1" t="s">
+      <c r="N64" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L64" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M64" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N64" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>142</v>
       </c>
@@ -4762,29 +4972,32 @@
       <c r="G65" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H65" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H65" s="1"/>
       <c r="I65" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="J65" s="8" t="s">
+      <c r="L65" s="1"/>
+      <c r="M65" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K65" s="1" t="s">
+      <c r="N65" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L65" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M65" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N65" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q65" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>143</v>
       </c>
@@ -4804,29 +5017,32 @@
       <c r="G66" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H66" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H66" s="1"/>
       <c r="I66" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J66" s="1" t="s">
+      <c r="L66" s="1"/>
+      <c r="M66" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="K66" s="1" t="s">
+      <c r="N66" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L66" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M66" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N66" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q66" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>145</v>
       </c>
@@ -4846,29 +5062,32 @@
       <c r="G67" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H67" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H67" s="1"/>
       <c r="I67" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J67" s="1" t="s">
+      <c r="L67" s="1"/>
+      <c r="M67" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="K67" s="1" t="s">
+      <c r="N67" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="L67" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M67" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N67" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q67" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>147</v>
       </c>
@@ -4888,29 +5107,32 @@
       <c r="G68" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H68" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H68" s="1"/>
       <c r="I68" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="J68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L68" s="1" t="s">
+      <c r="L68" s="1"/>
+      <c r="M68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O68" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="M68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N68" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q68" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>149</v>
       </c>
@@ -4930,30 +5152,33 @@
       <c r="G69" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="H69" s="1"/>
+      <c r="I69" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I69" s="1" t="s">
+      <c r="J69" s="1"/>
+      <c r="K69" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="J69" s="8" t="s">
+      <c r="L69" s="1"/>
+      <c r="M69" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K69" s="1" t="s">
+      <c r="N69" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L69" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M69" s="1" t="s">
+      <c r="O69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P69" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="N69" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="O69" s="4"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q69" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="R69" s="4"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>153</v>
       </c>
@@ -4973,29 +5198,32 @@
       <c r="G70" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="H70" s="1"/>
+      <c r="I70" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I70" s="1" t="s">
+      <c r="J70" s="1"/>
+      <c r="K70" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="J70" s="8" t="s">
+      <c r="L70" s="1"/>
+      <c r="M70" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K70" s="1" t="s">
+      <c r="N70" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L70" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M70" s="1" t="s">
+      <c r="O70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P70" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="N70" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q70" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>154</v>
       </c>
@@ -5015,29 +5243,32 @@
       <c r="G71" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H71" s="1" t="s">
+      <c r="H71" s="1"/>
+      <c r="I71" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I71" s="1" t="s">
+      <c r="J71" s="1"/>
+      <c r="K71" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J71" s="8" t="s">
+      <c r="L71" s="1"/>
+      <c r="M71" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K71" s="1" t="s">
+      <c r="N71" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L71" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M71" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N71" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q71" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>158</v>
       </c>
@@ -5057,29 +5288,32 @@
       <c r="G72" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H72" s="1" t="s">
+      <c r="H72" s="1"/>
+      <c r="I72" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I72" s="1" t="s">
+      <c r="J72" s="1"/>
+      <c r="K72" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J72" s="8" t="s">
+      <c r="L72" s="1"/>
+      <c r="M72" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K72" s="1" t="s">
+      <c r="N72" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L72" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M72" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N72" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O72" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P72" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q72" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>160</v>
       </c>
@@ -5099,29 +5333,32 @@
       <c r="G73" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H73" s="1" t="s">
+      <c r="H73" s="1"/>
+      <c r="I73" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I73" s="1" t="s">
+      <c r="J73" s="1"/>
+      <c r="K73" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J73" s="8" t="s">
+      <c r="L73" s="1"/>
+      <c r="M73" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K73" s="1" t="s">
+      <c r="N73" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L73" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M73" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N73" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q73" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>162</v>
       </c>
@@ -5141,29 +5378,32 @@
       <c r="G74" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H74" s="1" t="s">
+      <c r="H74" s="1"/>
+      <c r="I74" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I74" s="1" t="s">
+      <c r="J74" s="1"/>
+      <c r="K74" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J74" s="8" t="s">
+      <c r="L74" s="1"/>
+      <c r="M74" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K74" s="1" t="s">
+      <c r="N74" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="L74" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M74" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N74" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>164</v>
       </c>
@@ -5183,29 +5423,32 @@
       <c r="G75" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H75" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H75" s="1"/>
       <c r="I75" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J75" s="1" t="s">
+      <c r="L75" s="1"/>
+      <c r="M75" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="K75" s="1" t="s">
+      <c r="N75" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="L75" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M75" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N75" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q75" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>166</v>
       </c>
@@ -5225,29 +5468,32 @@
       <c r="G76" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H76" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H76" s="1"/>
       <c r="I76" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J76" s="1" t="s">
+      <c r="L76" s="1"/>
+      <c r="M76" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="K76" s="1" t="s">
+      <c r="N76" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="L76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N76" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q76" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>167</v>
       </c>
@@ -5267,30 +5513,33 @@
       <c r="G77" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H77" s="1" t="s">
-        <v>172</v>
-      </c>
+      <c r="H77" s="1"/>
       <c r="I77" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J77" s="1" t="s">
+      <c r="L77" s="1"/>
+      <c r="M77" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="K77" s="1" t="s">
+      <c r="N77" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="L77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N77" s="1" t="s">
+      <c r="O77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q77" s="1" t="s">
         <v>218</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N77">
+  <sortState ref="A2:Q77">
     <sortCondition ref="A2:A77"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
19T to 20T mapping adding dimension item uids for technical area, num or denom, and disagg type
</commit_message>
<xml_diff>
--- a/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
+++ b/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/site_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E550A91F-7C3B-294C-A162-B00AE18455B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EC9E6588-ABC7-5F4C-BF1D-F6F4B35F5E64}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1368" uniqueCount="384">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1596" uniqueCount="473">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -1185,13 +1185,280 @@
   </si>
   <si>
     <t>disagg_type_uid</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV7</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV8</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV9</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV10</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV11</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV12</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV13</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV14</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV15</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV16</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV17</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV18</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV19</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV20</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV21</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV22</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV23</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV24</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV25</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV26</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV27</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV28</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV29</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV30</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV31</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV32</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV33</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV34</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV35</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV36</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV37</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV38</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV39</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV40</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV41</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV42</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV43</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV44</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV45</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV46</t>
+  </si>
+  <si>
+    <t>Som9NRMQqV47</t>
+  </si>
+  <si>
+    <t>QpNj0nSuEhD</t>
+  </si>
+  <si>
+    <t>vw3VoiA4D0s</t>
+  </si>
+  <si>
+    <t>f5IPTM7mieH</t>
+  </si>
+  <si>
+    <t>NYAJ6QkEKbC</t>
+  </si>
+  <si>
+    <t>Uo2vBxak9im</t>
+  </si>
+  <si>
+    <t>lYTgCwEjUX6</t>
+  </si>
+  <si>
+    <t>RxyNwEV3oQf</t>
+  </si>
+  <si>
+    <t>AaCcy7dVfWw</t>
+  </si>
+  <si>
+    <t>cwZbCmUvjp7</t>
+  </si>
+  <si>
+    <t>BTIqHnjeG7l</t>
+  </si>
+  <si>
+    <t>Fvs28dwjL6e</t>
+  </si>
+  <si>
+    <t>gma5vVZgK49</t>
+  </si>
+  <si>
+    <t>Z6TU9Os82Yw</t>
+  </si>
+  <si>
+    <t>FfxbuFZVAM5</t>
+  </si>
+  <si>
+    <t>rI3JlpiuwEK</t>
+  </si>
+  <si>
+    <t>MvszPTQrUhy</t>
+  </si>
+  <si>
+    <t>udCop657yzi</t>
+  </si>
+  <si>
+    <t>bZOF8bon1dD</t>
+  </si>
+  <si>
+    <t>tOiM2uxcnkj</t>
+  </si>
+  <si>
+    <t>wdoUps1qb3V</t>
+  </si>
+  <si>
+    <t>hGUykTtC0Xm</t>
+  </si>
+  <si>
+    <t>fNQC7f36jre</t>
+  </si>
+  <si>
+    <t>KMhxXDjVseT</t>
+  </si>
+  <si>
+    <t>h0pvSVe1TYf</t>
+  </si>
+  <si>
+    <t>k2U2MDOywGj</t>
+  </si>
+  <si>
+    <t>Qbz6SrpmJ1y</t>
+  </si>
+  <si>
+    <t>CXO3RZgYCAY</t>
+  </si>
+  <si>
+    <t>pxz2gGSIQhG</t>
+  </si>
+  <si>
+    <t>Ua8iy6NgQks</t>
+  </si>
+  <si>
+    <t>iPfNX6Ylqp1</t>
+  </si>
+  <si>
+    <t>zzNslrLngKi</t>
+  </si>
+  <si>
+    <t>xds87opkbem</t>
+  </si>
+  <si>
+    <t>p6j1mfN4rjP</t>
+  </si>
+  <si>
+    <t>OoC9KSMqBms</t>
+  </si>
+  <si>
+    <t>oLVJbdHt6ou</t>
+  </si>
+  <si>
+    <t>UkvLXoUn0wG</t>
+  </si>
+  <si>
+    <t>jEpJPF6IVVB</t>
+  </si>
+  <si>
+    <t>z5IOTPUto8L</t>
+  </si>
+  <si>
+    <t>werJlVT6sf3</t>
+  </si>
+  <si>
+    <t>Lhk8mjk6Yk2</t>
+  </si>
+  <si>
+    <t>E3VaSq4JOzd</t>
+  </si>
+  <si>
+    <t>iFlQUEQcsfZ</t>
+  </si>
+  <si>
+    <t>dmPR3N6lKPJ</t>
+  </si>
+  <si>
+    <t>sdHeplyj1SL</t>
+  </si>
+  <si>
+    <t>kkfFCChSw4k</t>
+  </si>
+  <si>
+    <t>dcaYk7TXk4E</t>
+  </si>
+  <si>
+    <t>HlEDNiLt5hq</t>
+  </si>
+  <si>
+    <t>QEpxdKlM3zh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1335,6 +1602,18 @@
     <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF333399"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF1A1AA6"/>
       <name val="Courier New"/>
       <family val="1"/>
     </font>
@@ -1686,7 +1965,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1696,6 +1975,8 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2053,8 +2334,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2062,6 +2343,7 @@
     <col min="1" max="1" width="67.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29.33203125" customWidth="1"/>
     <col min="18" max="18" width="13.1640625" bestFit="1" customWidth="1"/>
@@ -2117,7 +2399,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -2137,15 +2419,21 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="10" t="s">
+        <v>426</v>
+      </c>
       <c r="I2" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="9" t="s">
+        <v>384</v>
+      </c>
       <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="L2" s="10" t="s">
+        <v>472</v>
+      </c>
       <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2162,7 +2450,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2182,15 +2470,21 @@
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="10" t="s">
+        <v>426</v>
+      </c>
       <c r="I3" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="9" t="s">
+        <v>385</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="1"/>
+      <c r="L3" s="10" t="s">
+        <v>472</v>
+      </c>
       <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2207,7 +2501,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -2227,15 +2521,21 @@
       <c r="G4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I4" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="9" t="s">
+        <v>386</v>
+      </c>
       <c r="K4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="10" t="s">
+        <v>456</v>
+      </c>
       <c r="M4" s="1" t="s">
         <v>213</v>
       </c>
@@ -2252,7 +2552,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -2272,15 +2572,21 @@
       <c r="G5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I5" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="9" t="s">
+        <v>387</v>
+      </c>
       <c r="K5" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="L5" s="1"/>
+      <c r="L5" s="10" t="s">
+        <v>456</v>
+      </c>
       <c r="M5" s="1" t="s">
         <v>213</v>
       </c>
@@ -2297,7 +2603,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2317,15 +2623,21 @@
       <c r="G6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I6" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="9" t="s">
+        <v>388</v>
+      </c>
       <c r="K6" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="L6" s="10" t="s">
+        <v>455</v>
+      </c>
       <c r="M6" s="1" t="s">
         <v>213</v>
       </c>
@@ -2342,7 +2654,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -2362,15 +2674,21 @@
       <c r="G7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I7" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="9" t="s">
+        <v>389</v>
+      </c>
       <c r="K7" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="L7" s="1"/>
+      <c r="L7" s="10" t="s">
+        <v>455</v>
+      </c>
       <c r="M7" s="1" t="s">
         <v>213</v>
       </c>
@@ -2387,7 +2705,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -2407,15 +2725,21 @@
       <c r="G8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="10" t="s">
+        <v>445</v>
+      </c>
       <c r="I8" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="9" t="s">
+        <v>390</v>
+      </c>
       <c r="K8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="10" t="s">
+        <v>451</v>
+      </c>
       <c r="M8" s="1" t="s">
         <v>211</v>
       </c>
@@ -2432,7 +2756,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2452,15 +2776,21 @@
       <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="10" t="s">
+        <v>445</v>
+      </c>
       <c r="I9" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J9" s="1"/>
+      <c r="J9" s="9" t="s">
+        <v>391</v>
+      </c>
       <c r="K9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="1"/>
+      <c r="L9" s="10" t="s">
+        <v>451</v>
+      </c>
       <c r="M9" s="1" t="s">
         <v>211</v>
       </c>
@@ -2477,7 +2807,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -2497,15 +2827,21 @@
       <c r="G10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I10" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="9" t="s">
+        <v>392</v>
+      </c>
       <c r="K10" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="L10" s="1"/>
+      <c r="L10" s="10" t="s">
+        <v>454</v>
+      </c>
       <c r="M10" s="1" t="s">
         <v>213</v>
       </c>
@@ -2522,7 +2858,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -2542,15 +2878,21 @@
       <c r="G11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I11" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="9" t="s">
+        <v>393</v>
+      </c>
       <c r="K11" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="L11" s="1"/>
+      <c r="L11" s="10" t="s">
+        <v>454</v>
+      </c>
       <c r="M11" s="1" t="s">
         <v>213</v>
       </c>
@@ -2567,7 +2909,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -2587,15 +2929,21 @@
       <c r="G12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I12" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="1"/>
+      <c r="J12" s="9" t="s">
+        <v>394</v>
+      </c>
       <c r="K12" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L12" s="1"/>
+      <c r="L12" s="10" t="s">
+        <v>457</v>
+      </c>
       <c r="M12" s="1" t="s">
         <v>213</v>
       </c>
@@ -2612,7 +2960,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -2632,15 +2980,21 @@
       <c r="G13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I13" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J13" s="1"/>
+      <c r="J13" s="9" t="s">
+        <v>395</v>
+      </c>
       <c r="K13" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L13" s="1"/>
+      <c r="L13" s="10" t="s">
+        <v>457</v>
+      </c>
       <c r="M13" s="1" t="s">
         <v>213</v>
       </c>
@@ -2657,7 +3011,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -2677,15 +3031,21 @@
       <c r="G14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I14" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="9" t="s">
+        <v>396</v>
+      </c>
       <c r="K14" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="L14" s="1"/>
+      <c r="L14" s="10" t="s">
+        <v>461</v>
+      </c>
       <c r="M14" s="5" t="s">
         <v>215</v>
       </c>
@@ -2702,7 +3062,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -2722,15 +3082,21 @@
       <c r="G15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I15" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J15" s="1"/>
+      <c r="J15" s="9" t="s">
+        <v>397</v>
+      </c>
       <c r="K15" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="L15" s="1"/>
+      <c r="L15" s="10" t="s">
+        <v>461</v>
+      </c>
       <c r="M15" s="5" t="s">
         <v>215</v>
       </c>
@@ -2747,7 +3113,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -2767,15 +3133,21 @@
       <c r="G16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I16" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="9" t="s">
+        <v>398</v>
+      </c>
       <c r="K16" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="L16" s="1"/>
+      <c r="L16" s="10" t="s">
+        <v>461</v>
+      </c>
       <c r="M16" s="1" t="s">
         <v>213</v>
       </c>
@@ -2792,7 +3164,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -2812,15 +3184,21 @@
       <c r="G17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I17" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J17" s="1"/>
+      <c r="J17" s="9" t="s">
+        <v>399</v>
+      </c>
       <c r="K17" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="L17" s="1"/>
+      <c r="L17" s="10" t="s">
+        <v>461</v>
+      </c>
       <c r="M17" s="1" t="s">
         <v>213</v>
       </c>
@@ -2837,7 +3215,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -2857,15 +3235,21 @@
       <c r="G18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I18" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="9" t="s">
+        <v>400</v>
+      </c>
       <c r="K18" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="L18" s="1"/>
+      <c r="L18" s="10" t="s">
+        <v>464</v>
+      </c>
       <c r="M18" s="1" t="s">
         <v>213</v>
       </c>
@@ -2882,7 +3266,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
@@ -2902,15 +3286,21 @@
       <c r="G19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I19" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="J19" s="9" t="s">
+        <v>401</v>
+      </c>
       <c r="K19" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="L19" s="1"/>
+      <c r="L19" s="10" t="s">
+        <v>464</v>
+      </c>
       <c r="M19" s="1" t="s">
         <v>213</v>
       </c>
@@ -2927,7 +3317,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -2947,15 +3337,21 @@
       <c r="G20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="1"/>
+      <c r="H20" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I20" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="9" t="s">
+        <v>402</v>
+      </c>
       <c r="K20" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="L20" s="1"/>
+      <c r="L20" s="10" t="s">
+        <v>465</v>
+      </c>
       <c r="M20" s="1" t="s">
         <v>213</v>
       </c>
@@ -2972,7 +3368,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
@@ -2992,15 +3388,21 @@
       <c r="G21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H21" s="1"/>
+      <c r="H21" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I21" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="J21" s="9" t="s">
+        <v>403</v>
+      </c>
       <c r="K21" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="L21" s="1"/>
+      <c r="L21" s="10" t="s">
+        <v>465</v>
+      </c>
       <c r="M21" s="1" t="s">
         <v>213</v>
       </c>
@@ -3017,7 +3419,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
@@ -3037,15 +3439,21 @@
       <c r="G22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I22" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J22" s="1"/>
+      <c r="J22" s="9" t="s">
+        <v>404</v>
+      </c>
       <c r="K22" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L22" s="1"/>
+      <c r="L22" s="10" t="s">
+        <v>466</v>
+      </c>
       <c r="M22" s="1" t="s">
         <v>215</v>
       </c>
@@ -3062,7 +3470,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>59</v>
       </c>
@@ -3082,15 +3490,21 @@
       <c r="G23" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I23" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J23" s="1"/>
+      <c r="J23" s="9" t="s">
+        <v>405</v>
+      </c>
       <c r="K23" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L23" s="1"/>
+      <c r="L23" s="10" t="s">
+        <v>466</v>
+      </c>
       <c r="M23" s="1" t="s">
         <v>215</v>
       </c>
@@ -3107,7 +3521,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -3127,15 +3541,21 @@
       <c r="G24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="1"/>
+      <c r="H24" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I24" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J24" s="1"/>
+      <c r="J24" s="9" t="s">
+        <v>406</v>
+      </c>
       <c r="K24" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="L24" s="1"/>
+      <c r="L24" s="10" t="s">
+        <v>467</v>
+      </c>
       <c r="M24" s="1" t="s">
         <v>213</v>
       </c>
@@ -3152,7 +3572,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
@@ -3172,15 +3592,21 @@
       <c r="G25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H25" s="1"/>
+      <c r="H25" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I25" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J25" s="1"/>
+      <c r="J25" s="9" t="s">
+        <v>407</v>
+      </c>
       <c r="K25" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="L25" s="1"/>
+      <c r="L25" s="10" t="s">
+        <v>467</v>
+      </c>
       <c r="M25" s="1" t="s">
         <v>213</v>
       </c>
@@ -3197,7 +3623,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
@@ -3217,15 +3643,21 @@
       <c r="G26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H26" s="1"/>
+      <c r="H26" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I26" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J26" s="1"/>
+      <c r="J26" s="9" t="s">
+        <v>408</v>
+      </c>
       <c r="K26" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="L26" s="1"/>
+      <c r="L26" s="10" t="s">
+        <v>469</v>
+      </c>
       <c r="M26" s="1" t="s">
         <v>213</v>
       </c>
@@ -3242,7 +3674,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
@@ -3262,15 +3694,21 @@
       <c r="G27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H27" s="1"/>
+      <c r="H27" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I27" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J27" s="1"/>
+      <c r="J27" s="9" t="s">
+        <v>409</v>
+      </c>
       <c r="K27" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="L27" s="1"/>
+      <c r="L27" s="10" t="s">
+        <v>469</v>
+      </c>
       <c r="M27" s="1" t="s">
         <v>213</v>
       </c>
@@ -3287,7 +3725,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>66</v>
       </c>
@@ -3307,15 +3745,21 @@
       <c r="G28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="1"/>
+      <c r="H28" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I28" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="9" t="s">
+        <v>410</v>
+      </c>
       <c r="K28" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="L28" s="1"/>
+      <c r="L28" s="10" t="s">
+        <v>470</v>
+      </c>
       <c r="M28" s="1" t="s">
         <v>213</v>
       </c>
@@ -3332,7 +3776,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
@@ -3352,15 +3796,21 @@
       <c r="G29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H29" s="1"/>
+      <c r="H29" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I29" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J29" s="1"/>
+      <c r="J29" s="9" t="s">
+        <v>411</v>
+      </c>
       <c r="K29" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="L29" s="1"/>
+      <c r="L29" s="10" t="s">
+        <v>470</v>
+      </c>
       <c r="M29" s="1" t="s">
         <v>213</v>
       </c>
@@ -3377,7 +3827,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>69</v>
       </c>
@@ -3397,15 +3847,21 @@
       <c r="G30" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H30" s="1"/>
+      <c r="H30" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I30" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J30" s="1"/>
+      <c r="J30" s="9" t="s">
+        <v>412</v>
+      </c>
       <c r="K30" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L30" s="1"/>
+      <c r="L30" s="10" t="s">
+        <v>471</v>
+      </c>
       <c r="M30" s="1" t="s">
         <v>213</v>
       </c>
@@ -3422,7 +3878,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>71</v>
       </c>
@@ -3442,15 +3898,21 @@
       <c r="G31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="1"/>
+      <c r="H31" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I31" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J31" s="1"/>
+      <c r="J31" s="9" t="s">
+        <v>413</v>
+      </c>
       <c r="K31" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L31" s="1"/>
+      <c r="L31" s="10" t="s">
+        <v>471</v>
+      </c>
       <c r="M31" s="1" t="s">
         <v>213</v>
       </c>
@@ -3467,7 +3929,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
@@ -3487,15 +3949,21 @@
       <c r="G32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="1"/>
+      <c r="H32" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I32" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J32" s="1"/>
+      <c r="J32" s="9" t="s">
+        <v>414</v>
+      </c>
       <c r="K32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L32" s="1"/>
+      <c r="L32" s="10" t="s">
+        <v>460</v>
+      </c>
       <c r="M32" s="1" t="s">
         <v>9</v>
       </c>
@@ -3512,7 +3980,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>75</v>
       </c>
@@ -3532,15 +4000,21 @@
       <c r="G33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H33" s="1"/>
+      <c r="H33" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I33" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J33" s="1"/>
+      <c r="J33" s="9" t="s">
+        <v>415</v>
+      </c>
       <c r="K33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L33" s="1"/>
+      <c r="L33" s="10" t="s">
+        <v>460</v>
+      </c>
       <c r="M33" s="1" t="s">
         <v>9</v>
       </c>
@@ -3557,7 +4031,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
@@ -3577,15 +4051,21 @@
       <c r="G34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H34" s="1"/>
+      <c r="H34" s="10" t="s">
+        <v>428</v>
+      </c>
       <c r="I34" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J34" s="1"/>
+      <c r="J34" s="9" t="s">
+        <v>416</v>
+      </c>
       <c r="K34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L34" s="1"/>
+      <c r="L34" s="10" t="s">
+        <v>468</v>
+      </c>
       <c r="M34" s="1" t="s">
         <v>9</v>
       </c>
@@ -3602,7 +4082,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>79</v>
       </c>
@@ -3622,15 +4102,21 @@
       <c r="G35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H35" s="1"/>
+      <c r="H35" s="10" t="s">
+        <v>429</v>
+      </c>
       <c r="I35" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J35" s="1"/>
+      <c r="J35" s="9" t="s">
+        <v>417</v>
+      </c>
       <c r="K35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L35" s="1"/>
+      <c r="L35" s="10" t="s">
+        <v>458</v>
+      </c>
       <c r="M35" s="1" t="s">
         <v>9</v>
       </c>
@@ -3647,7 +4133,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
@@ -3667,15 +4153,21 @@
       <c r="G36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H36" s="1"/>
+      <c r="H36" s="10" t="s">
+        <v>430</v>
+      </c>
       <c r="I36" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J36" s="1"/>
+      <c r="J36" s="9" t="s">
+        <v>418</v>
+      </c>
       <c r="K36" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="L36" s="1"/>
+      <c r="L36" s="10" t="s">
+        <v>463</v>
+      </c>
       <c r="M36" s="1" t="s">
         <v>9</v>
       </c>
@@ -3692,7 +4184,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
@@ -3712,15 +4204,21 @@
       <c r="G37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="1"/>
+      <c r="H37" s="10" t="s">
+        <v>431</v>
+      </c>
       <c r="I37" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J37" s="1"/>
+      <c r="J37" s="9" t="s">
+        <v>419</v>
+      </c>
       <c r="K37" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L37" s="1"/>
+      <c r="L37" s="10" t="s">
+        <v>450</v>
+      </c>
       <c r="M37" s="1" t="s">
         <v>353</v>
       </c>
@@ -3737,7 +4235,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>89</v>
       </c>
@@ -3757,15 +4255,21 @@
       <c r="G38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H38" s="1"/>
+      <c r="H38" s="10" t="s">
+        <v>431</v>
+      </c>
       <c r="I38" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J38" s="1"/>
+      <c r="J38" s="9" t="s">
+        <v>420</v>
+      </c>
       <c r="K38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L38" s="1"/>
+      <c r="L38" s="10" t="s">
+        <v>450</v>
+      </c>
       <c r="M38" s="1" t="s">
         <v>353</v>
       </c>
@@ -3782,7 +4286,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>91</v>
       </c>
@@ -3802,15 +4306,21 @@
       <c r="G39" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H39" s="1"/>
+      <c r="H39" s="10" t="s">
+        <v>432</v>
+      </c>
       <c r="I39" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J39" s="1"/>
+      <c r="J39" s="9" t="s">
+        <v>421</v>
+      </c>
       <c r="K39" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="L39" s="1"/>
+      <c r="L39" s="10" t="s">
+        <v>462</v>
+      </c>
       <c r="M39" s="1" t="s">
         <v>9</v>
       </c>
@@ -3827,7 +4337,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>95</v>
       </c>
@@ -3847,15 +4357,21 @@
       <c r="G40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H40" s="1"/>
+      <c r="H40" s="10" t="s">
+        <v>432</v>
+      </c>
       <c r="I40" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J40" s="1"/>
+      <c r="J40" s="9" t="s">
+        <v>422</v>
+      </c>
       <c r="K40" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="L40" s="1"/>
+      <c r="L40" s="10" t="s">
+        <v>462</v>
+      </c>
       <c r="M40" s="1" t="s">
         <v>9</v>
       </c>
@@ -3872,7 +4388,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
@@ -3892,15 +4408,21 @@
       <c r="G41" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H41" s="1"/>
+      <c r="H41" s="10" t="s">
+        <v>433</v>
+      </c>
       <c r="I41" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J41" s="1"/>
+      <c r="J41" s="9" t="s">
+        <v>423</v>
+      </c>
       <c r="K41" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L41" s="1"/>
+      <c r="L41" s="10" t="s">
+        <v>446</v>
+      </c>
       <c r="M41" s="1" t="s">
         <v>221</v>
       </c>
@@ -3917,7 +4439,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>101</v>
       </c>
@@ -3937,15 +4459,21 @@
       <c r="G42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H42" s="1"/>
+      <c r="H42" s="10" t="s">
+        <v>433</v>
+      </c>
       <c r="I42" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J42" s="1"/>
+      <c r="J42" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K42" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L42" s="1"/>
+      <c r="L42" s="10" t="s">
+        <v>446</v>
+      </c>
       <c r="M42" s="7" t="s">
         <v>222</v>
       </c>
@@ -3962,7 +4490,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>103</v>
       </c>
@@ -3982,15 +4510,21 @@
       <c r="G43" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H43" s="1"/>
+      <c r="H43" s="10" t="s">
+        <v>434</v>
+      </c>
       <c r="I43" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J43" s="1"/>
+      <c r="J43" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="K43" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L43" s="1"/>
+      <c r="L43" s="10" t="s">
+        <v>450</v>
+      </c>
       <c r="M43" s="1" t="s">
         <v>211</v>
       </c>
@@ -4007,7 +4541,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>106</v>
       </c>
@@ -4027,15 +4561,21 @@
       <c r="G44" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H44" s="1"/>
+      <c r="H44" s="10" t="s">
+        <v>434</v>
+      </c>
       <c r="I44" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J44" s="1"/>
+      <c r="J44" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K44" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L44" s="1"/>
+      <c r="L44" s="10" t="s">
+        <v>453</v>
+      </c>
       <c r="M44" s="1" t="s">
         <v>211</v>
       </c>
@@ -4052,7 +4592,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>109</v>
       </c>
@@ -4072,15 +4612,21 @@
       <c r="G45" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H45" s="1"/>
+      <c r="H45" s="10" t="s">
+        <v>434</v>
+      </c>
       <c r="I45" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J45" s="1"/>
+      <c r="J45" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K45" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L45" s="1"/>
+      <c r="L45" s="10" t="s">
+        <v>453</v>
+      </c>
       <c r="M45" s="1" t="s">
         <v>211</v>
       </c>
@@ -4097,7 +4643,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>110</v>
       </c>
@@ -4117,15 +4663,21 @@
       <c r="G46" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H46" s="1"/>
+      <c r="H46" s="10" t="s">
+        <v>434</v>
+      </c>
       <c r="I46" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J46" s="1"/>
+      <c r="J46" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K46" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L46" s="1"/>
+      <c r="L46" s="10" t="s">
+        <v>453</v>
+      </c>
       <c r="M46" s="1" t="s">
         <v>211</v>
       </c>
@@ -4142,7 +4694,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>111</v>
       </c>
@@ -4162,15 +4714,21 @@
       <c r="G47" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H47" s="1"/>
+      <c r="H47" s="10" t="s">
+        <v>435</v>
+      </c>
       <c r="I47" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J47" s="1"/>
+      <c r="J47" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K47" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L47" s="1"/>
+      <c r="L47" s="10" t="s">
+        <v>450</v>
+      </c>
       <c r="M47" s="1" t="s">
         <v>211</v>
       </c>
@@ -4187,7 +4745,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>113</v>
       </c>
@@ -4207,15 +4765,21 @@
       <c r="G48" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H48" s="1"/>
+      <c r="H48" s="10" t="s">
+        <v>436</v>
+      </c>
       <c r="I48" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J48" s="1"/>
+      <c r="J48" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K48" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L48" s="1"/>
+      <c r="L48" s="10" t="s">
+        <v>450</v>
+      </c>
       <c r="M48" s="1" t="s">
         <v>224</v>
       </c>
@@ -4232,7 +4796,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>115</v>
       </c>
@@ -4252,15 +4816,21 @@
       <c r="G49" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H49" s="1"/>
+      <c r="H49" s="10" t="s">
+        <v>436</v>
+      </c>
       <c r="I49" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J49" s="1"/>
+      <c r="J49" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L49" s="1"/>
+      <c r="L49" s="10" t="s">
+        <v>458</v>
+      </c>
       <c r="M49" s="1" t="s">
         <v>9</v>
       </c>
@@ -4277,7 +4847,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>116</v>
       </c>
@@ -4297,15 +4867,21 @@
       <c r="G50" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H50" s="1"/>
+      <c r="H50" s="10" t="s">
+        <v>436</v>
+      </c>
       <c r="I50" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J50" s="1"/>
+      <c r="J50" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K50" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L50" s="1"/>
+      <c r="L50" s="10" t="s">
+        <v>450</v>
+      </c>
       <c r="M50" s="1" t="s">
         <v>224</v>
       </c>
@@ -4322,7 +4898,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>118</v>
       </c>
@@ -4342,15 +4918,21 @@
       <c r="G51" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H51" s="1"/>
+      <c r="H51" s="10" t="s">
+        <v>436</v>
+      </c>
       <c r="I51" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J51" s="1"/>
+      <c r="J51" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K51" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L51" s="1"/>
+      <c r="L51" s="10" t="s">
+        <v>458</v>
+      </c>
       <c r="M51" s="1" t="s">
         <v>9</v>
       </c>
@@ -4367,7 +4949,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>119</v>
       </c>
@@ -4387,15 +4969,21 @@
       <c r="G52" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H52" s="1"/>
+      <c r="H52" s="10" t="s">
+        <v>437</v>
+      </c>
       <c r="I52" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J52" s="1"/>
+      <c r="J52" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K52" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L52" s="1"/>
+      <c r="L52" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M52" s="8" t="s">
         <v>360</v>
       </c>
@@ -4412,7 +5000,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>122</v>
       </c>
@@ -4432,15 +5020,21 @@
       <c r="G53" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H53" s="1"/>
+      <c r="H53" s="10" t="s">
+        <v>437</v>
+      </c>
       <c r="I53" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J53" s="1"/>
+      <c r="J53" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K53" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L53" s="1"/>
+      <c r="L53" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M53" s="8" t="s">
         <v>360</v>
       </c>
@@ -4457,7 +5051,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>123</v>
       </c>
@@ -4477,15 +5071,21 @@
       <c r="G54" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H54" s="1"/>
+      <c r="H54" s="10" t="s">
+        <v>438</v>
+      </c>
       <c r="I54" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J54" s="1"/>
+      <c r="J54" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="K54" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L54" s="1"/>
+      <c r="L54" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M54" s="8" t="s">
         <v>360</v>
       </c>
@@ -4502,7 +5102,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>127</v>
       </c>
@@ -4522,15 +5122,21 @@
       <c r="G55" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H55" s="1"/>
+      <c r="H55" s="10" t="s">
+        <v>438</v>
+      </c>
       <c r="I55" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J55" s="1"/>
+      <c r="J55" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="K55" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L55" s="1"/>
+      <c r="L55" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M55" s="8" t="s">
         <v>360</v>
       </c>
@@ -4547,7 +5153,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>129</v>
       </c>
@@ -4567,15 +5173,21 @@
       <c r="G56" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H56" s="1"/>
+      <c r="H56" s="10" t="s">
+        <v>438</v>
+      </c>
       <c r="I56" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J56" s="1"/>
+      <c r="J56" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="K56" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L56" s="1"/>
+      <c r="L56" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M56" s="8" t="s">
         <v>360</v>
       </c>
@@ -4592,7 +5204,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>131</v>
       </c>
@@ -4612,15 +5224,21 @@
       <c r="G57" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H57" s="1"/>
+      <c r="H57" s="10" t="s">
+        <v>438</v>
+      </c>
       <c r="I57" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J57" s="1"/>
+      <c r="J57" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="K57" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L57" s="1"/>
+      <c r="L57" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M57" s="8" t="s">
         <v>360</v>
       </c>
@@ -4637,7 +5255,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>133</v>
       </c>
@@ -4657,15 +5275,21 @@
       <c r="G58" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H58" s="1"/>
+      <c r="H58" s="10" t="s">
+        <v>438</v>
+      </c>
       <c r="I58" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J58" s="1"/>
+      <c r="J58" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K58" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L58" s="1"/>
+      <c r="L58" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M58" s="8" t="s">
         <v>360</v>
       </c>
@@ -4682,7 +5306,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>134</v>
       </c>
@@ -4702,15 +5326,21 @@
       <c r="G59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H59" s="1"/>
+      <c r="H59" s="10" t="s">
+        <v>438</v>
+      </c>
       <c r="I59" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J59" s="1"/>
+      <c r="J59" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K59" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L59" s="1"/>
+      <c r="L59" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M59" s="8" t="s">
         <v>360</v>
       </c>
@@ -4727,7 +5357,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>135</v>
       </c>
@@ -4747,15 +5377,21 @@
       <c r="G60" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H60" s="1"/>
+      <c r="H60" s="10" t="s">
+        <v>438</v>
+      </c>
       <c r="I60" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J60" s="1"/>
+      <c r="J60" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K60" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L60" s="1"/>
+      <c r="L60" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M60" s="8" t="s">
         <v>360</v>
       </c>
@@ -4772,7 +5408,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>136</v>
       </c>
@@ -4792,15 +5428,21 @@
       <c r="G61" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H61" s="1"/>
+      <c r="H61" s="10" t="s">
+        <v>438</v>
+      </c>
       <c r="I61" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J61" s="1"/>
+      <c r="J61" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K61" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L61" s="1"/>
+      <c r="L61" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M61" s="8" t="s">
         <v>360</v>
       </c>
@@ -4817,7 +5459,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>137</v>
       </c>
@@ -4837,15 +5479,21 @@
       <c r="G62" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H62" s="1"/>
+      <c r="H62" s="10" t="s">
+        <v>439</v>
+      </c>
       <c r="I62" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J62" s="1"/>
+      <c r="J62" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="K62" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L62" s="1"/>
+      <c r="L62" s="10" t="s">
+        <v>447</v>
+      </c>
       <c r="M62" s="8" t="s">
         <v>360</v>
       </c>
@@ -4862,7 +5510,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>139</v>
       </c>
@@ -4882,15 +5530,21 @@
       <c r="G63" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H63" s="1"/>
+      <c r="H63" s="10" t="s">
+        <v>439</v>
+      </c>
       <c r="I63" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J63" s="1"/>
+      <c r="J63" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K63" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L63" s="1"/>
+      <c r="L63" s="10" t="s">
+        <v>447</v>
+      </c>
       <c r="M63" s="8" t="s">
         <v>360</v>
       </c>
@@ -4907,7 +5561,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>141</v>
       </c>
@@ -4927,15 +5581,21 @@
       <c r="G64" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H64" s="1"/>
+      <c r="H64" s="10" t="s">
+        <v>439</v>
+      </c>
       <c r="I64" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J64" s="1"/>
+      <c r="J64" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K64" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L64" s="1"/>
+      <c r="L64" s="10" t="s">
+        <v>447</v>
+      </c>
       <c r="M64" s="8" t="s">
         <v>360</v>
       </c>
@@ -4952,7 +5612,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>142</v>
       </c>
@@ -4972,15 +5632,21 @@
       <c r="G65" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H65" s="1"/>
+      <c r="H65" s="10" t="s">
+        <v>439</v>
+      </c>
       <c r="I65" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J65" s="1"/>
+      <c r="J65" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K65" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L65" s="1"/>
+      <c r="L65" s="10" t="s">
+        <v>447</v>
+      </c>
       <c r="M65" s="8" t="s">
         <v>360</v>
       </c>
@@ -4997,7 +5663,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>143</v>
       </c>
@@ -5017,15 +5683,21 @@
       <c r="G66" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H66" s="1"/>
+      <c r="H66" s="10" t="s">
+        <v>440</v>
+      </c>
       <c r="I66" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J66" s="1"/>
+      <c r="J66" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L66" s="1"/>
+      <c r="L66" s="10" t="s">
+        <v>452</v>
+      </c>
       <c r="M66" s="1" t="s">
         <v>361</v>
       </c>
@@ -5042,7 +5714,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>145</v>
       </c>
@@ -5062,15 +5734,21 @@
       <c r="G67" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H67" s="1"/>
+      <c r="H67" s="10" t="s">
+        <v>441</v>
+      </c>
       <c r="I67" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J67" s="1"/>
+      <c r="J67" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K67" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L67" s="1"/>
+      <c r="L67" s="10" t="s">
+        <v>452</v>
+      </c>
       <c r="M67" s="1" t="s">
         <v>361</v>
       </c>
@@ -5087,7 +5765,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>147</v>
       </c>
@@ -5107,15 +5785,21 @@
       <c r="G68" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H68" s="1"/>
+      <c r="H68" s="10" t="s">
+        <v>441</v>
+      </c>
       <c r="I68" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J68" s="1"/>
+      <c r="J68" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K68" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="L68" s="1"/>
+      <c r="L68" s="10" t="s">
+        <v>459</v>
+      </c>
       <c r="M68" s="1" t="s">
         <v>9</v>
       </c>
@@ -5132,7 +5816,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>149</v>
       </c>
@@ -5152,15 +5836,21 @@
       <c r="G69" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H69" s="1"/>
+      <c r="H69" s="10" t="s">
+        <v>442</v>
+      </c>
       <c r="I69" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J69" s="1"/>
+      <c r="J69" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="K69" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="L69" s="1"/>
+      <c r="L69" s="10" t="s">
+        <v>449</v>
+      </c>
       <c r="M69" s="8" t="s">
         <v>360</v>
       </c>
@@ -5178,7 +5868,7 @@
       </c>
       <c r="R69" s="4"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>153</v>
       </c>
@@ -5198,15 +5888,21 @@
       <c r="G70" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H70" s="1"/>
+      <c r="H70" s="10" t="s">
+        <v>442</v>
+      </c>
       <c r="I70" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J70" s="1"/>
+      <c r="J70" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="K70" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="L70" s="1"/>
+      <c r="L70" s="10" t="s">
+        <v>449</v>
+      </c>
       <c r="M70" s="8" t="s">
         <v>360</v>
       </c>
@@ -5223,7 +5919,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>154</v>
       </c>
@@ -5243,15 +5939,21 @@
       <c r="G71" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H71" s="1"/>
+      <c r="H71" s="10" t="s">
+        <v>443</v>
+      </c>
       <c r="I71" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J71" s="1"/>
+      <c r="J71" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="K71" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L71" s="1"/>
+      <c r="L71" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M71" s="8" t="s">
         <v>360</v>
       </c>
@@ -5268,7 +5970,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>158</v>
       </c>
@@ -5288,15 +5990,21 @@
       <c r="G72" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H72" s="1"/>
+      <c r="H72" s="10" t="s">
+        <v>443</v>
+      </c>
       <c r="I72" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J72" s="1"/>
+      <c r="J72" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="K72" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L72" s="1"/>
+      <c r="L72" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M72" s="8" t="s">
         <v>360</v>
       </c>
@@ -5313,7 +6021,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>160</v>
       </c>
@@ -5333,15 +6041,21 @@
       <c r="G73" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H73" s="1"/>
+      <c r="H73" s="10" t="s">
+        <v>443</v>
+      </c>
       <c r="I73" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J73" s="1"/>
+      <c r="J73" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="K73" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L73" s="1"/>
+      <c r="L73" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M73" s="8" t="s">
         <v>360</v>
       </c>
@@ -5358,7 +6072,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>162</v>
       </c>
@@ -5378,15 +6092,21 @@
       <c r="G74" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H74" s="1"/>
+      <c r="H74" s="10" t="s">
+        <v>443</v>
+      </c>
       <c r="I74" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J74" s="1"/>
+      <c r="J74" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="K74" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L74" s="1"/>
+      <c r="L74" s="10" t="s">
+        <v>448</v>
+      </c>
       <c r="M74" s="8" t="s">
         <v>360</v>
       </c>
@@ -5403,7 +6123,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>164</v>
       </c>
@@ -5423,15 +6143,21 @@
       <c r="G75" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H75" s="1"/>
+      <c r="H75" s="10" t="s">
+        <v>444</v>
+      </c>
       <c r="I75" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J75" s="1"/>
+      <c r="J75" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K75" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L75" s="1"/>
+      <c r="L75" s="10" t="s">
+        <v>450</v>
+      </c>
       <c r="M75" s="1" t="s">
         <v>211</v>
       </c>
@@ -5448,7 +6174,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>166</v>
       </c>
@@ -5468,15 +6194,21 @@
       <c r="G76" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H76" s="1"/>
+      <c r="H76" s="10" t="s">
+        <v>444</v>
+      </c>
       <c r="I76" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J76" s="1"/>
+      <c r="J76" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K76" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L76" s="1"/>
+      <c r="L76" s="10" t="s">
+        <v>450</v>
+      </c>
       <c r="M76" s="1" t="s">
         <v>211</v>
       </c>
@@ -5493,7 +6225,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>167</v>
       </c>
@@ -5513,15 +6245,21 @@
       <c r="G77" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H77" s="1"/>
+      <c r="H77" s="10" t="s">
+        <v>444</v>
+      </c>
       <c r="I77" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J77" s="1"/>
+      <c r="J77" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="K77" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L77" s="1"/>
+      <c r="L77" s="10" t="s">
+        <v>450</v>
+      </c>
       <c r="M77" s="1" t="s">
         <v>211</v>
       </c>
@@ -5539,8 +6277,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q77">
-    <sortCondition ref="A2:A77"/>
+  <sortState ref="A2:R78">
+    <sortCondition ref="A2:A78"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove 2 empty columns
</commit_message>
<xml_diff>
--- a/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
+++ b/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/site_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EC9E6588-ABC7-5F4C-BF1D-F6F4B35F5E64}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{59D437C8-13B8-F740-BAF5-522E5E2323DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -1965,12 +1965,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -2332,10 +2331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R77"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:AQ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2343,13 +2342,12 @@
     <col min="1" max="1" width="67.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.33203125" customWidth="1"/>
-    <col min="18" max="18" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>374</v>
       </c>
@@ -2365,41 +2363,41 @@
       <c r="E1" t="s">
         <v>377</v>
       </c>
+      <c r="F1" t="s">
+        <v>204</v>
+      </c>
       <c r="G1" t="s">
-        <v>204</v>
+        <v>381</v>
       </c>
       <c r="H1" t="s">
-        <v>381</v>
+        <v>205</v>
       </c>
       <c r="I1" t="s">
-        <v>205</v>
+        <v>382</v>
       </c>
       <c r="J1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="K1" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="L1" t="s">
-        <v>383</v>
+        <v>207</v>
       </c>
       <c r="M1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="N1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="O1" t="s">
-        <v>209</v>
+        <v>378</v>
       </c>
       <c r="P1" t="s">
-        <v>378</v>
-      </c>
-      <c r="Q1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -2415,25 +2413,27 @@
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="H2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="K2" s="9" t="s">
         <v>472</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2441,16 +2441,13 @@
         <v>9</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>9</v>
+        <v>225</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q2" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2466,25 +2463,27 @@
       <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J3" s="9" t="s">
+      <c r="H3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>472</v>
       </c>
+      <c r="L3" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="M3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2492,16 +2491,13 @@
         <v>9</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>9</v>
+        <v>226</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q3" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -2517,42 +2513,41 @@
       <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J4" s="9" t="s">
+      <c r="H4" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="K4" s="9" t="s">
         <v>456</v>
       </c>
+      <c r="L4" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M4" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>9</v>
+        <v>371</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="Q4" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -2568,42 +2563,41 @@
       <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J5" s="9" t="s">
+      <c r="H5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>456</v>
       </c>
+      <c r="L5" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M5" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>9</v>
+        <v>372</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="Q5" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2619,42 +2613,41 @@
       <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J6" s="9" t="s">
+      <c r="H6" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="K6" s="9" t="s">
         <v>455</v>
       </c>
+      <c r="L6" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M6" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>9</v>
+        <v>371</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="Q6" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -2670,42 +2663,41 @@
       <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J7" s="9" t="s">
+      <c r="H7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="K7" s="9" t="s">
         <v>455</v>
       </c>
+      <c r="L7" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M7" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>9</v>
+        <v>372</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="Q7" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -2721,42 +2713,41 @@
       <c r="E8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J8" s="9" t="s">
+      <c r="H8" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="K8" s="9" t="s">
         <v>451</v>
       </c>
+      <c r="L8" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="M8" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>9</v>
+        <v>228</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q8" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2772,42 +2763,41 @@
       <c r="E9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J9" s="9" t="s">
+      <c r="H9" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="K9" s="9" t="s">
         <v>451</v>
       </c>
+      <c r="L9" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="M9" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>9</v>
+        <v>229</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q9" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -2823,42 +2813,41 @@
       <c r="E10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J10" s="9" t="s">
+      <c r="H10" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="K10" s="9" t="s">
         <v>454</v>
       </c>
+      <c r="L10" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M10" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>9</v>
+        <v>350</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q10" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -2874,42 +2863,41 @@
       <c r="E11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J11" s="9" t="s">
+      <c r="H11" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="K11" s="9" t="s">
         <v>454</v>
       </c>
+      <c r="L11" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M11" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>9</v>
+        <v>351</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q11" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -2925,42 +2913,41 @@
       <c r="E12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J12" s="9" t="s">
+      <c r="H12" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="K12" s="9" t="s">
         <v>457</v>
       </c>
+      <c r="L12" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M12" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>9</v>
+        <v>350</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q12" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -2976,42 +2963,41 @@
       <c r="E13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J13" s="9" t="s">
+      <c r="H13" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="K13" s="9" t="s">
         <v>457</v>
       </c>
+      <c r="L13" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M13" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>9</v>
+        <v>351</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q13" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -3027,42 +3013,41 @@
       <c r="E14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J14" s="9" t="s">
+      <c r="H14" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="K14" s="9" t="s">
         <v>461</v>
       </c>
+      <c r="L14" s="4" t="s">
+        <v>215</v>
+      </c>
       <c r="M14" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="N14" s="6" t="s">
         <v>216</v>
       </c>
+      <c r="N14" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="O14" s="1" t="s">
-        <v>9</v>
+        <v>350</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q14" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -3078,42 +3063,41 @@
       <c r="E15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="G15" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J15" s="9" t="s">
+      <c r="H15" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="K15" s="9" t="s">
         <v>461</v>
       </c>
+      <c r="L15" s="4" t="s">
+        <v>215</v>
+      </c>
       <c r="M15" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="N15" s="6" t="s">
         <v>216</v>
       </c>
+      <c r="N15" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="O15" s="1" t="s">
-        <v>9</v>
+        <v>351</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q15" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -3129,42 +3113,41 @@
       <c r="E16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J16" s="9" t="s">
+      <c r="H16" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="K16" s="9" t="s">
         <v>461</v>
       </c>
+      <c r="L16" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M16" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>9</v>
+        <v>350</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q16" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -3180,42 +3163,41 @@
       <c r="E17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="G17" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J17" s="9" t="s">
+      <c r="H17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="L17" s="10" t="s">
+      <c r="K17" s="9" t="s">
         <v>461</v>
       </c>
+      <c r="L17" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M17" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>9</v>
+        <v>351</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q17" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -3231,42 +3213,41 @@
       <c r="E18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J18" s="9" t="s">
+      <c r="H18" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="K18" s="9" t="s">
         <v>464</v>
       </c>
+      <c r="L18" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M18" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>9</v>
+        <v>350</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q18" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
@@ -3282,42 +3263,41 @@
       <c r="E19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="G19" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J19" s="9" t="s">
+      <c r="H19" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="L19" s="10" t="s">
+      <c r="K19" s="9" t="s">
         <v>464</v>
       </c>
+      <c r="L19" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M19" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>9</v>
+        <v>351</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q19" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -3333,42 +3313,41 @@
       <c r="E20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="G20" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J20" s="9" t="s">
+      <c r="H20" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="L20" s="10" t="s">
+      <c r="K20" s="9" t="s">
         <v>465</v>
       </c>
+      <c r="L20" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M20" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>9</v>
+        <v>350</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q20" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
@@ -3384,42 +3363,41 @@
       <c r="E21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J21" s="9" t="s">
+      <c r="H21" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="L21" s="10" t="s">
+      <c r="K21" s="9" t="s">
         <v>465</v>
       </c>
+      <c r="L21" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M21" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>9</v>
+        <v>351</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q21" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
@@ -3435,42 +3413,41 @@
       <c r="E22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="G22" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J22" s="9" t="s">
+      <c r="H22" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L22" s="10" t="s">
+      <c r="K22" s="9" t="s">
         <v>466</v>
       </c>
+      <c r="L22" s="1" t="s">
+        <v>215</v>
+      </c>
       <c r="M22" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>216</v>
+        <v>9</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>9</v>
+        <v>350</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q22" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>59</v>
       </c>
@@ -3486,42 +3463,41 @@
       <c r="E23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="G23" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J23" s="9" t="s">
+      <c r="H23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>405</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="L23" s="10" t="s">
+      <c r="K23" s="9" t="s">
         <v>466</v>
       </c>
+      <c r="L23" s="1" t="s">
+        <v>215</v>
+      </c>
       <c r="M23" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>216</v>
+        <v>9</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>9</v>
+        <v>351</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q23" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -3537,42 +3513,41 @@
       <c r="E24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="G24" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J24" s="9" t="s">
+      <c r="H24" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="L24" s="10" t="s">
+      <c r="K24" s="9" t="s">
         <v>467</v>
       </c>
+      <c r="L24" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M24" s="1" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>223</v>
+        <v>9</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>9</v>
+        <v>350</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q24" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
@@ -3588,42 +3563,41 @@
       <c r="E25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="G25" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J25" s="9" t="s">
+      <c r="H25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="L25" s="10" t="s">
+      <c r="K25" s="9" t="s">
         <v>467</v>
       </c>
+      <c r="L25" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M25" s="1" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>223</v>
+        <v>9</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>9</v>
+        <v>351</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q25" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
@@ -3639,42 +3613,41 @@
       <c r="E26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="G26" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J26" s="9" t="s">
+      <c r="H26" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I26" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="L26" s="10" t="s">
+      <c r="K26" s="9" t="s">
         <v>469</v>
       </c>
+      <c r="L26" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M26" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>9</v>
+        <v>350</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q26" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
@@ -3690,42 +3663,41 @@
       <c r="E27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="G27" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J27" s="9" t="s">
+      <c r="H27" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I27" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="L27" s="10" t="s">
+      <c r="K27" s="9" t="s">
         <v>469</v>
       </c>
+      <c r="L27" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M27" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>9</v>
+        <v>351</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q27" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>66</v>
       </c>
@@ -3741,42 +3713,41 @@
       <c r="E28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="G28" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J28" s="9" t="s">
+      <c r="H28" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I28" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="L28" s="10" t="s">
+      <c r="K28" s="9" t="s">
         <v>470</v>
       </c>
+      <c r="L28" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M28" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>9</v>
+        <v>350</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q28" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
@@ -3792,42 +3763,41 @@
       <c r="E29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="G29" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J29" s="9" t="s">
+      <c r="H29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I29" s="8" t="s">
         <v>411</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="L29" s="10" t="s">
+      <c r="K29" s="9" t="s">
         <v>470</v>
       </c>
+      <c r="L29" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M29" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>9</v>
+        <v>351</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q29" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>69</v>
       </c>
@@ -3843,42 +3813,41 @@
       <c r="E30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H30" s="10" t="s">
+      <c r="G30" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J30" s="9" t="s">
+      <c r="H30" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I30" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L30" s="10" t="s">
+      <c r="K30" s="9" t="s">
         <v>471</v>
       </c>
+      <c r="L30" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M30" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>9</v>
+        <v>350</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q30" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>71</v>
       </c>
@@ -3894,42 +3863,41 @@
       <c r="E31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="G31" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J31" s="9" t="s">
+      <c r="H31" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I31" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L31" s="10" t="s">
+      <c r="K31" s="9" t="s">
         <v>471</v>
       </c>
+      <c r="L31" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="M31" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>9</v>
+        <v>351</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q31" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
@@ -3945,42 +3913,41 @@
       <c r="E32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="G32" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J32" s="9" t="s">
+      <c r="H32" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I32" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L32" s="10" t="s">
+      <c r="K32" s="9" t="s">
         <v>460</v>
       </c>
+      <c r="L32" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="M32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>9</v>
+        <v>219</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>219</v>
+        <v>350</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q32" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>75</v>
       </c>
@@ -3996,42 +3963,41 @@
       <c r="E33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="G33" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="I33" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J33" s="9" t="s">
+      <c r="H33" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I33" s="8" t="s">
         <v>415</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L33" s="10" t="s">
+      <c r="K33" s="9" t="s">
         <v>460</v>
       </c>
+      <c r="L33" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="M33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>9</v>
+        <v>219</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>219</v>
+        <v>351</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q33" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
@@ -4047,42 +4013,41 @@
       <c r="E34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H34" s="10" t="s">
+      <c r="G34" s="9" t="s">
         <v>428</v>
       </c>
-      <c r="I34" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J34" s="9" t="s">
+      <c r="H34" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I34" s="8" t="s">
         <v>416</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L34" s="10" t="s">
+      <c r="K34" s="9" t="s">
         <v>468</v>
       </c>
+      <c r="L34" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="M34" s="1" t="s">
-        <v>9</v>
+        <v>212</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O34" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q34" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>79</v>
       </c>
@@ -4098,42 +4063,41 @@
       <c r="E35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H35" s="10" t="s">
+      <c r="G35" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="I35" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J35" s="9" t="s">
+      <c r="H35" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I35" s="8" t="s">
         <v>417</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L35" s="10" t="s">
+      <c r="K35" s="9" t="s">
         <v>458</v>
       </c>
+      <c r="L35" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="M35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>9</v>
+        <v>352</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>352</v>
+        <v>9</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q35" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
@@ -4149,25 +4113,27 @@
       <c r="E36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H36" s="10" t="s">
+      <c r="G36" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="I36" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J36" s="9" t="s">
+      <c r="H36" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I36" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="L36" s="10" t="s">
+      <c r="K36" s="9" t="s">
         <v>463</v>
       </c>
+      <c r="L36" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="M36" s="1" t="s">
         <v>9</v>
       </c>
@@ -4178,13 +4144,10 @@
         <v>9</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q36" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
@@ -4200,42 +4163,41 @@
       <c r="E37" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="10" t="s">
+      <c r="G37" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="I37" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J37" s="9" t="s">
+      <c r="H37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I37" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L37" s="10" t="s">
+      <c r="K37" s="9" t="s">
         <v>450</v>
       </c>
+      <c r="L37" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="M37" s="1" t="s">
-        <v>353</v>
+        <v>214</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q37" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>89</v>
       </c>
@@ -4251,42 +4213,41 @@
       <c r="E38" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H38" s="10" t="s">
+      <c r="G38" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J38" s="9" t="s">
+      <c r="H38" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I38" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L38" s="10" t="s">
+      <c r="K38" s="9" t="s">
         <v>450</v>
       </c>
+      <c r="L38" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="M38" s="1" t="s">
-        <v>353</v>
+        <v>214</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O38" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q38" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>91</v>
       </c>
@@ -4302,42 +4263,41 @@
       <c r="E39" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H39" s="10" t="s">
+      <c r="G39" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="I39" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J39" s="9" t="s">
+      <c r="H39" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I39" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="L39" s="10" t="s">
+      <c r="K39" s="9" t="s">
         <v>462</v>
       </c>
+      <c r="L39" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="M39" s="1" t="s">
-        <v>9</v>
+        <v>223</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>223</v>
+        <v>9</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>9</v>
+        <v>354</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="Q39" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>95</v>
       </c>
@@ -4353,42 +4313,41 @@
       <c r="E40" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H40" s="10" t="s">
+      <c r="G40" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="I40" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J40" s="9" t="s">
+      <c r="H40" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I40" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="L40" s="10" t="s">
+      <c r="K40" s="9" t="s">
         <v>462</v>
       </c>
+      <c r="L40" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="M40" s="1" t="s">
-        <v>9</v>
+        <v>223</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>223</v>
+        <v>9</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>9</v>
+        <v>355</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="Q40" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
@@ -4404,27 +4363,29 @@
       <c r="E41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="G41" s="9" t="s">
         <v>433</v>
       </c>
-      <c r="I41" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J41" s="9" t="s">
+      <c r="H41" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I41" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L41" s="10" t="s">
+      <c r="K41" s="9" t="s">
         <v>446</v>
       </c>
+      <c r="L41" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="M41" s="1" t="s">
-        <v>221</v>
+        <v>9</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>9</v>
@@ -4433,13 +4394,10 @@
         <v>9</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q41" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>101</v>
       </c>
@@ -4455,28 +4413,30 @@
       <c r="E42" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H42" s="10" t="s">
+      <c r="G42" s="9" t="s">
         <v>433</v>
       </c>
-      <c r="I42" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J42" s="9" t="s">
+      <c r="H42" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I42" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L42" s="10" t="s">
+      <c r="K42" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="M42" s="7" t="s">
+      <c r="L42" s="6" t="s">
         <v>222</v>
       </c>
+      <c r="M42" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="N42" s="1" t="s">
         <v>9</v>
       </c>
@@ -4484,13 +4444,10 @@
         <v>9</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q42" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>103</v>
       </c>
@@ -4506,42 +4463,41 @@
       <c r="E43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H43" s="10" t="s">
+      <c r="G43" s="9" t="s">
         <v>434</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J43" s="9" t="s">
+      <c r="I43" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L43" s="10" t="s">
+      <c r="K43" s="9" t="s">
         <v>450</v>
       </c>
+      <c r="L43" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="M43" s="1" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>223</v>
+        <v>9</v>
       </c>
       <c r="O43" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q43" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>106</v>
       </c>
@@ -4557,42 +4513,41 @@
       <c r="E44" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H44" s="10" t="s">
+      <c r="G44" s="9" t="s">
         <v>434</v>
       </c>
-      <c r="I44" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J44" s="9" t="s">
+      <c r="H44" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I44" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L44" s="10" t="s">
+      <c r="K44" s="9" t="s">
         <v>453</v>
       </c>
+      <c r="L44" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="M44" s="1" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P44" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O44" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="Q44" s="1" t="s">
+      <c r="P44" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>109</v>
       </c>
@@ -4608,42 +4563,41 @@
       <c r="E45" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H45" s="10" t="s">
+      <c r="G45" s="9" t="s">
         <v>434</v>
       </c>
-      <c r="I45" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J45" s="9" t="s">
+      <c r="H45" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I45" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L45" s="10" t="s">
+      <c r="K45" s="9" t="s">
         <v>453</v>
       </c>
+      <c r="L45" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="M45" s="1" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="O45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P45" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O45" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="Q45" s="1" t="s">
+      <c r="P45" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>110</v>
       </c>
@@ -4659,42 +4613,41 @@
       <c r="E46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H46" s="10" t="s">
+      <c r="G46" s="9" t="s">
         <v>434</v>
       </c>
-      <c r="I46" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J46" s="9" t="s">
+      <c r="H46" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I46" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L46" s="10" t="s">
+      <c r="K46" s="9" t="s">
         <v>453</v>
       </c>
+      <c r="L46" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="M46" s="1" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P46" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O46" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="Q46" s="1" t="s">
+      <c r="P46" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>111</v>
       </c>
@@ -4710,42 +4663,41 @@
       <c r="E47" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H47" s="10" t="s">
+      <c r="G47" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="I47" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J47" s="9" t="s">
+      <c r="H47" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I47" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L47" s="10" t="s">
+      <c r="K47" s="9" t="s">
         <v>450</v>
       </c>
+      <c r="L47" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="M47" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="O47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P47" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P47" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>113</v>
       </c>
@@ -4761,42 +4713,41 @@
       <c r="E48" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H48" s="10" t="s">
+      <c r="G48" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J48" s="9" t="s">
+      <c r="H48" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I48" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L48" s="10" t="s">
+      <c r="K48" s="9" t="s">
         <v>450</v>
       </c>
+      <c r="L48" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="M48" s="1" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O48" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q48" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>115</v>
       </c>
@@ -4812,42 +4763,41 @@
       <c r="E49" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H49" s="10" t="s">
+      <c r="G49" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="I49" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J49" s="9" t="s">
+      <c r="H49" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I49" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L49" s="10" t="s">
+      <c r="K49" s="9" t="s">
         <v>458</v>
       </c>
+      <c r="L49" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="M49" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>9</v>
+        <v>359</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>359</v>
+        <v>9</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q49" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>116</v>
       </c>
@@ -4863,42 +4813,41 @@
       <c r="E50" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H50" s="10" t="s">
+      <c r="G50" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="I50" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J50" s="9" t="s">
+      <c r="H50" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I50" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L50" s="10" t="s">
+      <c r="K50" s="9" t="s">
         <v>450</v>
       </c>
+      <c r="L50" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="M50" s="1" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="O50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P50" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O50" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P50" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>118</v>
       </c>
@@ -4914,42 +4863,41 @@
       <c r="E51" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H51" s="10" t="s">
+      <c r="G51" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="I51" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J51" s="9" t="s">
+      <c r="H51" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I51" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L51" s="10" t="s">
+      <c r="K51" s="9" t="s">
         <v>458</v>
       </c>
+      <c r="L51" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="M51" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>9</v>
+        <v>359</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>359</v>
+        <v>9</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q51" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>119</v>
       </c>
@@ -4965,42 +4913,41 @@
       <c r="E52" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H52" s="10" t="s">
+      <c r="G52" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="I52" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J52" s="9" t="s">
+      <c r="H52" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I52" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K52" s="1" t="s">
+      <c r="J52" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L52" s="10" t="s">
+      <c r="K52" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M52" s="8" t="s">
+      <c r="L52" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M52" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N52" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O52" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q52" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>122</v>
       </c>
@@ -5016,42 +4963,41 @@
       <c r="E53" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H53" s="10" t="s">
+      <c r="G53" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="I53" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J53" s="9" t="s">
+      <c r="H53" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I53" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="J53" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L53" s="10" t="s">
+      <c r="K53" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M53" s="8" t="s">
+      <c r="L53" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M53" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N53" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O53" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q53" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>123</v>
       </c>
@@ -5067,42 +5013,41 @@
       <c r="E54" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H54" s="10" t="s">
+      <c r="G54" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J54" s="9" t="s">
+      <c r="I54" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="J54" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L54" s="10" t="s">
+      <c r="K54" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M54" s="8" t="s">
+      <c r="L54" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M54" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N54" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O54" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q54" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>127</v>
       </c>
@@ -5118,42 +5063,41 @@
       <c r="E55" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H55" s="10" t="s">
+      <c r="G55" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="H55" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J55" s="9" t="s">
+      <c r="I55" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="J55" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L55" s="10" t="s">
+      <c r="K55" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M55" s="8" t="s">
+      <c r="L55" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M55" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N55" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O55" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q55" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>129</v>
       </c>
@@ -5169,42 +5113,41 @@
       <c r="E56" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H56" s="10" t="s">
+      <c r="G56" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="H56" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J56" s="9" t="s">
+      <c r="I56" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="K56" s="1" t="s">
+      <c r="J56" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L56" s="10" t="s">
+      <c r="K56" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M56" s="8" t="s">
+      <c r="L56" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M56" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N56" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O56" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q56" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>131</v>
       </c>
@@ -5220,42 +5163,41 @@
       <c r="E57" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H57" s="10" t="s">
+      <c r="G57" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="I57" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J57" s="9" t="s">
+      <c r="I57" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="K57" s="1" t="s">
+      <c r="J57" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L57" s="10" t="s">
+      <c r="K57" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M57" s="8" t="s">
+      <c r="L57" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M57" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N57" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O57" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q57" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>133</v>
       </c>
@@ -5271,42 +5213,41 @@
       <c r="E58" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H58" s="10" t="s">
+      <c r="G58" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="I58" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J58" s="9" t="s">
+      <c r="H58" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I58" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="J58" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L58" s="10" t="s">
+      <c r="K58" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M58" s="8" t="s">
+      <c r="L58" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M58" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N58" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O58" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q58" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>134</v>
       </c>
@@ -5322,42 +5263,41 @@
       <c r="E59" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H59" s="10" t="s">
+      <c r="G59" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="I59" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J59" s="9" t="s">
+      <c r="H59" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I59" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K59" s="1" t="s">
+      <c r="J59" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L59" s="10" t="s">
+      <c r="K59" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M59" s="8" t="s">
+      <c r="L59" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M59" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N59" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O59" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q59" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>135</v>
       </c>
@@ -5373,42 +5313,41 @@
       <c r="E60" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H60" s="10" t="s">
+      <c r="G60" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="I60" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J60" s="9" t="s">
+      <c r="H60" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I60" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="J60" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L60" s="10" t="s">
+      <c r="K60" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M60" s="8" t="s">
+      <c r="L60" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M60" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N60" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O60" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q60" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>136</v>
       </c>
@@ -5424,42 +5363,41 @@
       <c r="E61" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1" t="s">
+      <c r="F61" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H61" s="10" t="s">
+      <c r="G61" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="I61" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J61" s="9" t="s">
+      <c r="H61" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I61" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K61" s="1" t="s">
+      <c r="J61" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L61" s="10" t="s">
+      <c r="K61" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M61" s="8" t="s">
+      <c r="L61" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M61" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N61" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O61" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q61" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>137</v>
       </c>
@@ -5475,42 +5413,41 @@
       <c r="E62" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1" t="s">
+      <c r="F62" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H62" s="10" t="s">
+      <c r="G62" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="I62" s="1" t="s">
+      <c r="H62" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J62" s="9" t="s">
+      <c r="I62" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="K62" s="1" t="s">
+      <c r="J62" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L62" s="10" t="s">
+      <c r="K62" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="M62" s="8" t="s">
+      <c r="L62" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M62" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N62" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O62" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q62" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>139</v>
       </c>
@@ -5526,42 +5463,41 @@
       <c r="E63" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1" t="s">
+      <c r="F63" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H63" s="10" t="s">
+      <c r="G63" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="I63" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J63" s="9" t="s">
+      <c r="H63" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I63" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K63" s="1" t="s">
+      <c r="J63" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L63" s="10" t="s">
+      <c r="K63" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="M63" s="8" t="s">
+      <c r="L63" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M63" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N63" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O63" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P63" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q63" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>141</v>
       </c>
@@ -5577,42 +5513,41 @@
       <c r="E64" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1" t="s">
+      <c r="F64" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H64" s="10" t="s">
+      <c r="G64" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="I64" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J64" s="9" t="s">
+      <c r="H64" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I64" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K64" s="1" t="s">
+      <c r="J64" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L64" s="10" t="s">
+      <c r="K64" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="M64" s="8" t="s">
+      <c r="L64" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M64" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N64" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O64" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P64" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q64" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>142</v>
       </c>
@@ -5628,42 +5563,41 @@
       <c r="E65" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1" t="s">
+      <c r="F65" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H65" s="10" t="s">
+      <c r="G65" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="I65" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J65" s="9" t="s">
+      <c r="H65" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I65" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K65" s="1" t="s">
+      <c r="J65" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L65" s="10" t="s">
+      <c r="K65" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="M65" s="8" t="s">
+      <c r="L65" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M65" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N65" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O65" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q65" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>143</v>
       </c>
@@ -5679,42 +5613,41 @@
       <c r="E66" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1" t="s">
+      <c r="F66" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H66" s="10" t="s">
+      <c r="G66" s="9" t="s">
         <v>440</v>
       </c>
-      <c r="I66" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J66" s="9" t="s">
+      <c r="H66" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I66" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K66" s="1" t="s">
+      <c r="J66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L66" s="10" t="s">
+      <c r="K66" s="9" t="s">
         <v>452</v>
       </c>
+      <c r="L66" s="1" t="s">
+        <v>361</v>
+      </c>
       <c r="M66" s="1" t="s">
-        <v>361</v>
+        <v>214</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O66" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q66" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>145</v>
       </c>
@@ -5730,42 +5663,41 @@
       <c r="E67" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1" t="s">
+      <c r="F67" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H67" s="10" t="s">
+      <c r="G67" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="I67" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J67" s="9" t="s">
+      <c r="H67" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I67" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K67" s="1" t="s">
+      <c r="J67" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L67" s="10" t="s">
+      <c r="K67" s="9" t="s">
         <v>452</v>
       </c>
+      <c r="L67" s="1" t="s">
+        <v>361</v>
+      </c>
       <c r="M67" s="1" t="s">
-        <v>361</v>
+        <v>214</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="O67" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P67" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q67" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>147</v>
       </c>
@@ -5781,42 +5713,41 @@
       <c r="E68" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1" t="s">
+      <c r="F68" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H68" s="10" t="s">
+      <c r="G68" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="I68" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J68" s="9" t="s">
+      <c r="H68" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I68" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K68" s="1" t="s">
+      <c r="J68" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="L68" s="10" t="s">
+      <c r="K68" s="9" t="s">
         <v>459</v>
       </c>
+      <c r="L68" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="M68" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>9</v>
+        <v>219</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>219</v>
+        <v>9</v>
       </c>
       <c r="P68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q68" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>149</v>
       </c>
@@ -5832,43 +5763,41 @@
       <c r="E69" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1" t="s">
+      <c r="F69" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H69" s="10" t="s">
+      <c r="G69" s="9" t="s">
         <v>442</v>
       </c>
-      <c r="I69" s="1" t="s">
+      <c r="H69" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J69" s="9" t="s">
+      <c r="I69" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="K69" s="1" t="s">
+      <c r="J69" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="L69" s="10" t="s">
+      <c r="K69" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="M69" s="8" t="s">
+      <c r="L69" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M69" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N69" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>9</v>
+        <v>370</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="Q69" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="R69" s="4"/>
-    </row>
-    <row r="70" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>153</v>
       </c>
@@ -5884,42 +5813,41 @@
       <c r="E70" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1" t="s">
+      <c r="F70" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H70" s="10" t="s">
+      <c r="G70" s="9" t="s">
         <v>442</v>
       </c>
-      <c r="I70" s="1" t="s">
+      <c r="H70" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J70" s="9" t="s">
+      <c r="I70" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="K70" s="1" t="s">
+      <c r="J70" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="L70" s="10" t="s">
+      <c r="K70" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="M70" s="8" t="s">
+      <c r="L70" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M70" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N70" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>9</v>
+        <v>370</v>
       </c>
       <c r="P70" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="Q70" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>154</v>
       </c>
@@ -5935,42 +5863,41 @@
       <c r="E71" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1" t="s">
+      <c r="F71" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H71" s="10" t="s">
+      <c r="G71" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="I71" s="1" t="s">
+      <c r="H71" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J71" s="9" t="s">
+      <c r="I71" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="K71" s="1" t="s">
+      <c r="J71" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L71" s="10" t="s">
+      <c r="K71" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M71" s="8" t="s">
+      <c r="L71" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M71" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N71" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O71" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q71" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>158</v>
       </c>
@@ -5986,42 +5913,41 @@
       <c r="E72" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1" t="s">
+      <c r="F72" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H72" s="10" t="s">
+      <c r="G72" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="I72" s="1" t="s">
+      <c r="H72" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J72" s="9" t="s">
+      <c r="I72" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="K72" s="1" t="s">
+      <c r="J72" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L72" s="10" t="s">
+      <c r="K72" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M72" s="8" t="s">
+      <c r="L72" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M72" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N72" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O72" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q72" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>160</v>
       </c>
@@ -6037,42 +5963,41 @@
       <c r="E73" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1" t="s">
+      <c r="F73" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H73" s="10" t="s">
+      <c r="G73" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="I73" s="1" t="s">
+      <c r="H73" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J73" s="9" t="s">
+      <c r="I73" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="K73" s="1" t="s">
+      <c r="J73" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L73" s="10" t="s">
+      <c r="K73" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M73" s="8" t="s">
+      <c r="L73" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M73" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N73" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O73" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q73" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>162</v>
       </c>
@@ -6088,42 +6013,41 @@
       <c r="E74" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1" t="s">
+      <c r="F74" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="H74" s="10" t="s">
+      <c r="G74" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="I74" s="1" t="s">
+      <c r="H74" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J74" s="9" t="s">
+      <c r="I74" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="K74" s="1" t="s">
+      <c r="J74" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L74" s="10" t="s">
+      <c r="K74" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="M74" s="8" t="s">
+      <c r="L74" s="7" t="s">
         <v>360</v>
       </c>
+      <c r="M74" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N74" s="1" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="O74" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q74" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>164</v>
       </c>
@@ -6139,42 +6063,41 @@
       <c r="E75" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1" t="s">
+      <c r="F75" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H75" s="10" t="s">
+      <c r="G75" s="9" t="s">
         <v>444</v>
       </c>
-      <c r="I75" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J75" s="9" t="s">
+      <c r="H75" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I75" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K75" s="1" t="s">
+      <c r="J75" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L75" s="10" t="s">
+      <c r="K75" s="9" t="s">
         <v>450</v>
       </c>
+      <c r="L75" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="M75" s="1" t="s">
-        <v>211</v>
+        <v>373</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>373</v>
+        <v>9</v>
       </c>
       <c r="O75" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P75" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q75" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>166</v>
       </c>
@@ -6190,42 +6113,41 @@
       <c r="E76" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1" t="s">
+      <c r="F76" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H76" s="10" t="s">
+      <c r="G76" s="9" t="s">
         <v>444</v>
       </c>
-      <c r="I76" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J76" s="9" t="s">
+      <c r="H76" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I76" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K76" s="1" t="s">
+      <c r="J76" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L76" s="10" t="s">
+      <c r="K76" s="9" t="s">
         <v>450</v>
       </c>
+      <c r="L76" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="M76" s="1" t="s">
-        <v>211</v>
+        <v>373</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>373</v>
+        <v>9</v>
       </c>
       <c r="O76" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q76" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>167</v>
       </c>
@@ -6241,43 +6163,42 @@
       <c r="E77" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1" t="s">
+      <c r="F77" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H77" s="10" t="s">
+      <c r="G77" s="9" t="s">
         <v>444</v>
       </c>
-      <c r="I77" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J77" s="9" t="s">
+      <c r="H77" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I77" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="K77" s="1" t="s">
+      <c r="J77" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L77" s="10" t="s">
+      <c r="K77" s="9" t="s">
         <v>450</v>
       </c>
+      <c r="L77" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="M77" s="1" t="s">
-        <v>211</v>
+        <v>373</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>373</v>
+        <v>9</v>
       </c>
       <c r="O77" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q77" s="1" t="s">
         <v>218</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:R78">
+  <sortState ref="A2:P78">
     <sortCondition ref="A2:A78"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Map19Tto20T - fixing incorrect dimension item uids
</commit_message>
<xml_diff>
--- a/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
+++ b/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/site_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{59D437C8-13B8-F740-BAF5-522E5E2323DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{146F88BC-A891-6448-ACDB-6B2E6077CD9D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1596" uniqueCount="473">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1596" uniqueCount="433">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -1188,126 +1188,6 @@
   </si>
   <si>
     <t>Som9NRMQqV7</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV8</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV9</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV10</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV11</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV12</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV13</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV14</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV15</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV16</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV17</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV18</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV19</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV20</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV21</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV22</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV23</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV24</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV25</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV26</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV27</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV28</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV29</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV30</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV31</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV32</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV33</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV34</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV35</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV36</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV37</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV38</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV39</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV40</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV41</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV42</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV43</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV44</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV45</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV46</t>
-  </si>
-  <si>
-    <t>Som9NRMQqV47</t>
   </si>
   <si>
     <t>QpNj0nSuEhD</t>
@@ -2333,8 +2213,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:AQ1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2343,6 +2223,7 @@
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29.33203125" customWidth="1"/>
   </cols>
@@ -2417,19 +2298,19 @@
         <v>11</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>426</v>
+        <v>386</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="9" t="s">
         <v>384</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>472</v>
+        <v>432</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>9</v>
@@ -2467,19 +2348,19 @@
         <v>11</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>426</v>
+        <v>386</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>385</v>
+      <c r="I3" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>472</v>
+        <v>432</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>9</v>
@@ -2517,19 +2398,19 @@
         <v>73</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>386</v>
+      <c r="I4" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>196</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>456</v>
+        <v>416</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>213</v>
@@ -2567,19 +2448,19 @@
         <v>73</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>387</v>
+      <c r="I5" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>196</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>456</v>
+        <v>416</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>213</v>
@@ -2617,19 +2498,19 @@
         <v>73</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>388</v>
+      <c r="I6" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>182</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>455</v>
+        <v>415</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>213</v>
@@ -2667,19 +2548,19 @@
         <v>73</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>389</v>
+      <c r="I7" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>182</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>455</v>
+        <v>415</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>213</v>
@@ -2717,19 +2598,19 @@
         <v>31</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>445</v>
+        <v>405</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>390</v>
+      <c r="I8" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>451</v>
+        <v>411</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>211</v>
@@ -2767,19 +2648,19 @@
         <v>31</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>445</v>
+        <v>405</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>391</v>
+      <c r="I9" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>451</v>
+        <v>411</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>211</v>
@@ -2817,19 +2698,19 @@
         <v>73</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>392</v>
+      <c r="I10" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>186</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>454</v>
+        <v>414</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>213</v>
@@ -2867,19 +2748,19 @@
         <v>73</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I11" s="8" t="s">
-        <v>393</v>
+      <c r="I11" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>186</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>454</v>
+        <v>414</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>213</v>
@@ -2917,19 +2798,19 @@
         <v>73</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I12" s="8" t="s">
-        <v>394</v>
+      <c r="I12" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>199</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>457</v>
+        <v>417</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>213</v>
@@ -2967,19 +2848,19 @@
         <v>73</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>395</v>
+      <c r="I13" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>199</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>457</v>
+        <v>417</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>213</v>
@@ -3017,19 +2898,19 @@
         <v>73</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I14" s="8" t="s">
-        <v>396</v>
+      <c r="I14" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>197</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>215</v>
@@ -3067,19 +2948,19 @@
         <v>73</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I15" s="8" t="s">
-        <v>397</v>
+      <c r="I15" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>197</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>215</v>
@@ -3117,19 +2998,19 @@
         <v>73</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I16" s="8" t="s">
-        <v>398</v>
+      <c r="I16" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>177</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>213</v>
@@ -3167,19 +3048,19 @@
         <v>73</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>399</v>
+      <c r="I17" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>177</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>213</v>
@@ -3217,19 +3098,19 @@
         <v>73</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I18" s="8" t="s">
-        <v>400</v>
+      <c r="I18" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>193</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>464</v>
+        <v>424</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>213</v>
@@ -3267,19 +3148,19 @@
         <v>73</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I19" s="8" t="s">
-        <v>401</v>
+      <c r="I19" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>193</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>464</v>
+        <v>424</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>213</v>
@@ -3317,19 +3198,19 @@
         <v>73</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I20" s="8" t="s">
-        <v>402</v>
+      <c r="I20" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>179</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>465</v>
+        <v>425</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>213</v>
@@ -3367,19 +3248,19 @@
         <v>73</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>403</v>
+      <c r="I21" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>179</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>465</v>
+        <v>425</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>213</v>
@@ -3417,19 +3298,19 @@
         <v>73</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I22" s="8" t="s">
-        <v>404</v>
+      <c r="I22" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>190</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>466</v>
+        <v>426</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>215</v>
@@ -3467,19 +3348,19 @@
         <v>73</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I23" s="8" t="s">
-        <v>405</v>
+      <c r="I23" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>190</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>466</v>
+        <v>426</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>215</v>
@@ -3517,19 +3398,19 @@
         <v>73</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I24" s="8" t="s">
-        <v>406</v>
+      <c r="I24" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>194</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>467</v>
+        <v>427</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>213</v>
@@ -3567,19 +3448,19 @@
         <v>73</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I25" s="8" t="s">
-        <v>407</v>
+      <c r="I25" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>194</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>467</v>
+        <v>427</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>213</v>
@@ -3617,19 +3498,19 @@
         <v>73</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I26" s="8" t="s">
-        <v>408</v>
+      <c r="I26" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>188</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>469</v>
+        <v>429</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>213</v>
@@ -3667,19 +3548,19 @@
         <v>73</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I27" s="8" t="s">
-        <v>409</v>
+      <c r="I27" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>188</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>469</v>
+        <v>429</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>213</v>
@@ -3717,19 +3598,19 @@
         <v>73</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I28" s="8" t="s">
-        <v>410</v>
+      <c r="I28" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>202</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>470</v>
+        <v>430</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>213</v>
@@ -3767,19 +3648,19 @@
         <v>73</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>411</v>
+      <c r="I29" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>202</v>
       </c>
       <c r="K29" s="9" t="s">
-        <v>470</v>
+        <v>430</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>213</v>
@@ -3817,19 +3698,19 @@
         <v>73</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I30" s="8" t="s">
-        <v>412</v>
+      <c r="I30" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>183</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>471</v>
+        <v>431</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>213</v>
@@ -3867,19 +3748,19 @@
         <v>73</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>413</v>
+      <c r="I31" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>183</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>471</v>
+        <v>431</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>213</v>
@@ -3917,19 +3798,19 @@
         <v>73</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I32" s="8" t="s">
-        <v>414</v>
+      <c r="I32" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>74</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>9</v>
@@ -3967,19 +3848,19 @@
         <v>73</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I33" s="8" t="s">
-        <v>415</v>
+      <c r="I33" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>74</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>9</v>
@@ -4017,19 +3898,19 @@
         <v>77</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>428</v>
+        <v>388</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I34" s="8" t="s">
-        <v>416</v>
+      <c r="I34" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>468</v>
+        <v>428</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>9</v>
@@ -4067,19 +3948,19 @@
         <v>80</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>429</v>
+        <v>389</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I35" s="8" t="s">
-        <v>417</v>
+      <c r="I35" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>81</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>458</v>
+        <v>418</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>9</v>
@@ -4117,19 +3998,19 @@
         <v>83</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>430</v>
+        <v>390</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I36" s="8" t="s">
-        <v>418</v>
+      <c r="I36" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>181</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>463</v>
+        <v>423</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>9</v>
@@ -4167,19 +4048,19 @@
         <v>86</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>431</v>
+        <v>391</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I37" s="8" t="s">
-        <v>419</v>
+      <c r="I37" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>105</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>353</v>
@@ -4217,19 +4098,19 @@
         <v>86</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>431</v>
+        <v>391</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I38" s="8" t="s">
-        <v>420</v>
+      <c r="I38" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>105</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>353</v>
@@ -4267,19 +4148,19 @@
         <v>92</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>432</v>
+        <v>392</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="8" t="s">
-        <v>421</v>
+      <c r="I39" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>203</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>9</v>
@@ -4317,19 +4198,19 @@
         <v>92</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>432</v>
+        <v>392</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I40" s="8" t="s">
-        <v>422</v>
+      <c r="I40" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>203</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>9</v>
@@ -4367,19 +4248,19 @@
         <v>98</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>433</v>
+        <v>393</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I41" s="8" t="s">
-        <v>423</v>
+      <c r="I41" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>99</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>446</v>
+        <v>406</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>221</v>
@@ -4417,19 +4298,19 @@
         <v>98</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>433</v>
+        <v>393</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I42" s="8" t="s">
-        <v>424</v>
+      <c r="I42" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>99</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>446</v>
+        <v>406</v>
       </c>
       <c r="L42" s="6" t="s">
         <v>222</v>
@@ -4467,19 +4348,19 @@
         <v>104</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>434</v>
+        <v>394</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>105</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>211</v>
@@ -4517,19 +4398,19 @@
         <v>104</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>434</v>
+        <v>394</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I44" s="8" t="s">
-        <v>424</v>
+      <c r="I44" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>107</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>453</v>
+        <v>413</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>211</v>
@@ -4567,19 +4448,19 @@
         <v>104</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>434</v>
+        <v>394</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I45" s="8" t="s">
-        <v>424</v>
+      <c r="I45" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>107</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>453</v>
+        <v>413</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>211</v>
@@ -4617,19 +4498,19 @@
         <v>104</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>434</v>
+        <v>394</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I46" s="8" t="s">
-        <v>424</v>
+      <c r="I46" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>107</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>453</v>
+        <v>413</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>211</v>
@@ -4667,19 +4548,19 @@
         <v>112</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>435</v>
+        <v>395</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I47" s="8" t="s">
-        <v>424</v>
+      <c r="I47" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>105</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>211</v>
@@ -4717,19 +4598,19 @@
         <v>117</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>436</v>
+        <v>396</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I48" s="8" t="s">
-        <v>424</v>
+      <c r="I48" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>105</v>
       </c>
       <c r="K48" s="9" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>224</v>
@@ -4767,19 +4648,19 @@
         <v>117</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>436</v>
+        <v>396</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I49" s="8" t="s">
-        <v>424</v>
+      <c r="I49" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>81</v>
       </c>
       <c r="K49" s="9" t="s">
-        <v>458</v>
+        <v>418</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>9</v>
@@ -4817,19 +4698,19 @@
         <v>117</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>436</v>
+        <v>396</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I50" s="8" t="s">
-        <v>424</v>
+      <c r="I50" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>105</v>
       </c>
       <c r="K50" s="9" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>224</v>
@@ -4867,19 +4748,19 @@
         <v>117</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>436</v>
+        <v>396</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I51" s="8" t="s">
-        <v>424</v>
+      <c r="I51" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>81</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>458</v>
+        <v>418</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>9</v>
@@ -4917,19 +4798,19 @@
         <v>120</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>437</v>
+        <v>397</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I52" s="8" t="s">
-        <v>424</v>
+      <c r="I52" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L52" s="7" t="s">
         <v>360</v>
@@ -4967,19 +4848,19 @@
         <v>120</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>437</v>
+        <v>397</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I53" s="8" t="s">
-        <v>424</v>
+      <c r="I53" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K53" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L53" s="7" t="s">
         <v>360</v>
@@ -5017,19 +4898,19 @@
         <v>124</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>438</v>
+        <v>398</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L54" s="7" t="s">
         <v>360</v>
@@ -5067,19 +4948,19 @@
         <v>124</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>438</v>
+        <v>398</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K55" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L55" s="7" t="s">
         <v>360</v>
@@ -5117,19 +4998,19 @@
         <v>124</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>438</v>
+        <v>398</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L56" s="7" t="s">
         <v>360</v>
@@ -5167,19 +5048,19 @@
         <v>124</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>438</v>
+        <v>398</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L57" s="7" t="s">
         <v>360</v>
@@ -5217,19 +5098,19 @@
         <v>124</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>438</v>
+        <v>398</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I58" s="8" t="s">
-        <v>424</v>
+      <c r="I58" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K58" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L58" s="7" t="s">
         <v>360</v>
@@ -5267,19 +5148,19 @@
         <v>124</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>438</v>
+        <v>398</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I59" s="8" t="s">
-        <v>424</v>
+      <c r="I59" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K59" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L59" s="7" t="s">
         <v>360</v>
@@ -5317,19 +5198,19 @@
         <v>124</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>438</v>
+        <v>398</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I60" s="8" t="s">
-        <v>424</v>
+      <c r="I60" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K60" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L60" s="7" t="s">
         <v>360</v>
@@ -5367,19 +5248,19 @@
         <v>124</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>438</v>
+        <v>398</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I61" s="8" t="s">
-        <v>424</v>
+      <c r="I61" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K61" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L61" s="7" t="s">
         <v>360</v>
@@ -5417,19 +5298,19 @@
         <v>138</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>439</v>
+        <v>399</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>176</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>447</v>
+        <v>407</v>
       </c>
       <c r="L62" s="7" t="s">
         <v>360</v>
@@ -5467,19 +5348,19 @@
         <v>138</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>439</v>
+        <v>399</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I63" s="8" t="s">
-        <v>424</v>
+      <c r="I63" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>176</v>
       </c>
       <c r="K63" s="9" t="s">
-        <v>447</v>
+        <v>407</v>
       </c>
       <c r="L63" s="7" t="s">
         <v>360</v>
@@ -5517,19 +5398,19 @@
         <v>138</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>439</v>
+        <v>399</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I64" s="8" t="s">
-        <v>424</v>
+      <c r="I64" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>176</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>447</v>
+        <v>407</v>
       </c>
       <c r="L64" s="7" t="s">
         <v>360</v>
@@ -5567,19 +5448,19 @@
         <v>138</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>439</v>
+        <v>399</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I65" s="8" t="s">
-        <v>424</v>
+      <c r="I65" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>176</v>
       </c>
       <c r="K65" s="9" t="s">
-        <v>447</v>
+        <v>407</v>
       </c>
       <c r="L65" s="7" t="s">
         <v>360</v>
@@ -5617,19 +5498,19 @@
         <v>144</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>440</v>
+        <v>400</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I66" s="8" t="s">
-        <v>424</v>
+      <c r="I66" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K66" s="9" t="s">
-        <v>452</v>
+        <v>412</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>361</v>
@@ -5667,19 +5548,19 @@
         <v>146</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>441</v>
+        <v>401</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I67" s="8" t="s">
-        <v>424</v>
+      <c r="I67" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>452</v>
+        <v>412</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>361</v>
@@ -5717,19 +5598,19 @@
         <v>146</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>441</v>
+        <v>401</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I68" s="8" t="s">
-        <v>424</v>
+      <c r="I68" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>148</v>
       </c>
       <c r="K68" s="9" t="s">
-        <v>459</v>
+        <v>419</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>9</v>
@@ -5767,19 +5648,19 @@
         <v>150</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>442</v>
+        <v>402</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>175</v>
       </c>
       <c r="K69" s="9" t="s">
-        <v>449</v>
+        <v>409</v>
       </c>
       <c r="L69" s="7" t="s">
         <v>360</v>
@@ -5817,19 +5698,19 @@
         <v>150</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>442</v>
+        <v>402</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>175</v>
       </c>
       <c r="K70" s="9" t="s">
-        <v>449</v>
+        <v>409</v>
       </c>
       <c r="L70" s="7" t="s">
         <v>360</v>
@@ -5867,19 +5748,19 @@
         <v>155</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>443</v>
+        <v>403</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K71" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L71" s="7" t="s">
         <v>360</v>
@@ -5917,19 +5798,19 @@
         <v>155</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>443</v>
+        <v>403</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K72" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L72" s="7" t="s">
         <v>360</v>
@@ -5967,19 +5848,19 @@
         <v>155</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>443</v>
+        <v>403</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K73" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L73" s="7" t="s">
         <v>360</v>
@@ -6017,19 +5898,19 @@
         <v>155</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>443</v>
+        <v>403</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>170</v>
       </c>
       <c r="I74" s="8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>171</v>
       </c>
       <c r="K74" s="9" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="L74" s="7" t="s">
         <v>360</v>
@@ -6067,19 +5948,19 @@
         <v>165</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>444</v>
+        <v>404</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I75" s="8" t="s">
-        <v>424</v>
+      <c r="I75" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>105</v>
       </c>
       <c r="K75" s="9" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>211</v>
@@ -6117,19 +5998,19 @@
         <v>165</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>444</v>
+        <v>404</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I76" s="8" t="s">
-        <v>424</v>
+      <c r="I76" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>105</v>
       </c>
       <c r="K76" s="9" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>211</v>
@@ -6167,19 +6048,19 @@
         <v>165</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>444</v>
+        <v>404</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I77" s="8" t="s">
-        <v>424</v>
+      <c r="I77" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>105</v>
       </c>
       <c r="K77" s="9" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="L77" s="1" t="s">
         <v>211</v>

</xml_diff>

<commit_message>
Map19Tto20T correct a couple dimension item uids
</commit_message>
<xml_diff>
--- a/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
+++ b/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/site_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{146F88BC-A891-6448-ACDB-6B2E6077CD9D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7E6806E2-2A1D-4E4E-87E3-64730EA2C78E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1596" uniqueCount="433">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1596" uniqueCount="434">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -1332,6 +1332,9 @@
   </si>
   <si>
     <t>QEpxdKlM3zh</t>
+  </si>
+  <si>
+    <t>Qr9eyrVLHSg</t>
   </si>
 </sst>
 </file>
@@ -2213,8 +2216,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3010,7 +3013,7 @@
         <v>177</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>213</v>
@@ -3060,7 +3063,7 @@
         <v>177</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>213</v>

</xml_diff>

<commit_message>
19Tto20TMap - adding dx and pe columns
</commit_message>
<xml_diff>
--- a/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
+++ b/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/site_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7E6806E2-2A1D-4E4E-87E3-64730EA2C78E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{37187D7E-33A5-A640-AA96-301C33CE9988}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35720" yWindow="660" windowWidth="33600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1596" uniqueCount="434">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1598" uniqueCount="436">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -1335,6 +1335,12 @@
   </si>
   <si>
     <t>Qr9eyrVLHSg</t>
+  </si>
+  <si>
+    <t>dx</t>
+  </si>
+  <si>
+    <t>pe</t>
   </si>
 </sst>
 </file>
@@ -2214,10 +2220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P77"/>
+  <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2225,13 +2231,13 @@
     <col min="1" max="1" width="67.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>374</v>
       </c>
@@ -2248,40 +2254,46 @@
         <v>377</v>
       </c>
       <c r="F1" t="s">
+        <v>434</v>
+      </c>
+      <c r="G1" t="s">
         <v>204</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>381</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>205</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>382</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>379</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>383</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>435</v>
+      </c>
+      <c r="N1" t="s">
         <v>207</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>208</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>209</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>378</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -2297,41 +2309,43 @@
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="M2" s="9"/>
       <c r="N2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2347,41 +2361,43 @@
       <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="M3" s="9"/>
       <c r="N3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -2397,41 +2413,43 @@
       <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="9"/>
+      <c r="N4" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -2447,41 +2465,43 @@
       <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="L5" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="9"/>
+      <c r="N5" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2497,41 +2517,43 @@
       <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="L6" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="9"/>
+      <c r="N6" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -2547,41 +2569,43 @@
       <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="L7" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="9"/>
+      <c r="N7" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -2597,41 +2621,43 @@
       <c r="E8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J8" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="L8" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="9"/>
+      <c r="N8" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2647,41 +2673,43 @@
       <c r="E9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J9" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="L9" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="9"/>
+      <c r="N9" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -2697,41 +2725,43 @@
       <c r="E10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J10" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="L10" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="9"/>
+      <c r="N10" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -2747,41 +2777,43 @@
       <c r="E11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="H11" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J11" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="L11" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="9"/>
+      <c r="N11" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -2797,41 +2829,43 @@
       <c r="E12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="L12" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="9"/>
+      <c r="N12" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -2847,41 +2881,43 @@
       <c r="E13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J13" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="L13" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="9"/>
+      <c r="N13" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -2897,41 +2933,43 @@
       <c r="E14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J14" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="L14" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="M14" s="9"/>
+      <c r="N14" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="O14" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -2947,41 +2985,43 @@
       <c r="E15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="H15" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J15" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="L15" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="M15" s="9"/>
+      <c r="N15" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="O15" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q15" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -2997,41 +3037,43 @@
       <c r="E16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="H16" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J16" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="L16" s="9" t="s">
         <v>433</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="9"/>
+      <c r="N16" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O16" s="1" t="s">
+      <c r="P16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q16" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -3047,41 +3089,43 @@
       <c r="E17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="L17" s="9" t="s">
         <v>433</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="9"/>
+      <c r="N17" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q17" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -3097,41 +3141,43 @@
       <c r="E18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="H18" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J18" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="K18" s="9" t="s">
+      <c r="L18" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="9"/>
+      <c r="N18" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q18" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
@@ -3147,41 +3193,43 @@
       <c r="E19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="H19" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J19" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="K19" s="9" t="s">
+      <c r="L19" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="M19" s="9"/>
+      <c r="N19" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O19" s="1" t="s">
+      <c r="P19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q19" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="R19" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -3197,41 +3245,43 @@
       <c r="E20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="H20" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J20" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="K20" s="9" t="s">
+      <c r="L20" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="9"/>
+      <c r="N20" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O20" s="1" t="s">
+      <c r="P20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q20" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
@@ -3247,41 +3297,43 @@
       <c r="E21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="H21" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I21" s="9" t="s">
+      <c r="I21" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J21" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="L21" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="9"/>
+      <c r="N21" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O21" s="1" t="s">
+      <c r="P21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q21" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
@@ -3297,41 +3349,43 @@
       <c r="E22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="H22" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I22" s="9" t="s">
+      <c r="I22" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J22" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="L22" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="M22" s="9"/>
+      <c r="N22" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O22" s="1" t="s">
+      <c r="P22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q22" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="R22" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>59</v>
       </c>
@@ -3347,41 +3401,43 @@
       <c r="E23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="H23" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I23" s="9" t="s">
+      <c r="I23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J23" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="K23" s="9" t="s">
+      <c r="L23" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="M23" s="9"/>
+      <c r="N23" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O23" s="1" t="s">
+      <c r="P23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q23" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -3397,41 +3453,43 @@
       <c r="E24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I24" s="9" t="s">
+      <c r="I24" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J24" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="K24" s="9" t="s">
+      <c r="L24" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="M24" s="9"/>
+      <c r="N24" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="N24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O24" s="1" t="s">
+      <c r="P24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q24" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="R24" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
@@ -3447,41 +3505,43 @@
       <c r="E25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="H25" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I25" s="9" t="s">
+      <c r="I25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J25" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="K25" s="9" t="s">
+      <c r="L25" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="M25" s="9"/>
+      <c r="N25" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q25" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
@@ -3497,41 +3557,43 @@
       <c r="E26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="1"/>
+      <c r="G26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="H26" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J26" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="K26" s="9" t="s">
+      <c r="L26" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="M26" s="9"/>
+      <c r="N26" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O26" s="1" t="s">
+      <c r="P26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q26" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="P26" s="1" t="s">
+      <c r="R26" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
@@ -3547,41 +3609,43 @@
       <c r="E27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="H27" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J27" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="K27" s="9" t="s">
+      <c r="L27" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="M27" s="9"/>
+      <c r="N27" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O27" s="1" t="s">
+      <c r="P27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q27" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="R27" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>66</v>
       </c>
@@ -3597,41 +3661,43 @@
       <c r="E28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="1"/>
+      <c r="G28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="H28" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I28" s="9" t="s">
+      <c r="I28" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J28" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="K28" s="9" t="s">
+      <c r="L28" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="M28" s="9"/>
+      <c r="N28" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O28" s="1" t="s">
+      <c r="P28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q28" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="R28" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
@@ -3647,41 +3713,43 @@
       <c r="E29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="H29" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I29" s="9" t="s">
+      <c r="I29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J29" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="K29" s="9" t="s">
+      <c r="L29" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="M29" s="9"/>
+      <c r="N29" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O29" s="1" t="s">
+      <c r="P29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="R29" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>69</v>
       </c>
@@ -3697,41 +3765,43 @@
       <c r="E30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="1"/>
+      <c r="G30" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="H30" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J30" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="L30" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="M30" s="9"/>
+      <c r="N30" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O30" s="1" t="s">
+      <c r="P30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q30" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>71</v>
       </c>
@@ -3747,41 +3817,43 @@
       <c r="E31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="H31" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J31" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="K31" s="9" t="s">
+      <c r="L31" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="M31" s="9"/>
+      <c r="N31" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="O31" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O31" s="1" t="s">
+      <c r="P31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q31" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="P31" s="1" t="s">
+      <c r="R31" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
@@ -3797,41 +3869,43 @@
       <c r="E32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="1"/>
+      <c r="G32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="H32" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I32" s="9" t="s">
+      <c r="I32" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J32" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="L32" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="L32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="M32" s="9"/>
       <c r="N32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="Q32" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="P32" s="1" t="s">
+      <c r="R32" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>75</v>
       </c>
@@ -3847,41 +3921,43 @@
       <c r="E33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="1"/>
+      <c r="G33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="H33" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I33" s="9" t="s">
+      <c r="I33" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J33" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K33" s="9" t="s">
+      <c r="L33" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="L33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="M33" s="9"/>
       <c r="N33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P33" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="Q33" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="P33" s="1" t="s">
+      <c r="R33" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
@@ -3897,41 +3973,43 @@
       <c r="E34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="H34" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I34" s="9" t="s">
+      <c r="I34" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J34" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K34" s="9" t="s">
+      <c r="L34" s="9" t="s">
         <v>428</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M34" s="1" t="s">
+      <c r="M34" s="9"/>
+      <c r="N34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O34" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R34" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>79</v>
       </c>
@@ -3947,41 +4025,43 @@
       <c r="E35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="1"/>
+      <c r="G35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="H35" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J35" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K35" s="9" t="s">
+      <c r="L35" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="M35" s="9"/>
       <c r="N35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P35" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="O35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P35" s="1" t="s">
+      <c r="Q35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R35" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
@@ -3997,30 +4077,26 @@
       <c r="E36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="1"/>
+      <c r="G36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="H36" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I36" s="9" t="s">
+      <c r="I36" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J36" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="K36" s="9" t="s">
+      <c r="L36" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="L36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="M36" s="9"/>
       <c r="N36" s="1" t="s">
         <v>9</v>
       </c>
@@ -4028,10 +4104,16 @@
         <v>9</v>
       </c>
       <c r="P36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R36" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
@@ -4047,41 +4129,43 @@
       <c r="E37" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="1"/>
+      <c r="G37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="H37" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I37" s="9" t="s">
+      <c r="I37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J37" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K37" s="9" t="s">
+      <c r="L37" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="M37" s="9"/>
+      <c r="N37" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="O37" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R37" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>89</v>
       </c>
@@ -4097,41 +4181,43 @@
       <c r="E38" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="1"/>
+      <c r="G38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="H38" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I38" s="9" t="s">
+      <c r="I38" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J38" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K38" s="9" t="s">
+      <c r="L38" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="M38" s="9"/>
+      <c r="N38" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="O38" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R38" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>91</v>
       </c>
@@ -4147,41 +4233,43 @@
       <c r="E39" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="1"/>
+      <c r="G39" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="H39" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I39" s="9" t="s">
+      <c r="I39" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J39" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="K39" s="9" t="s">
+      <c r="L39" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M39" s="1" t="s">
+      <c r="M39" s="9"/>
+      <c r="N39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O39" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="N39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O39" s="1" t="s">
+      <c r="P39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q39" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="P39" s="1" t="s">
+      <c r="R39" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>95</v>
       </c>
@@ -4197,41 +4285,43 @@
       <c r="E40" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="1"/>
+      <c r="G40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="H40" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I40" s="9" t="s">
+      <c r="I40" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J40" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="K40" s="9" t="s">
+      <c r="L40" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M40" s="1" t="s">
+      <c r="M40" s="9"/>
+      <c r="N40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O40" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="N40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O40" s="1" t="s">
+      <c r="P40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q40" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="P40" s="1" t="s">
+      <c r="R40" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
@@ -4247,41 +4337,43 @@
       <c r="E41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" s="1"/>
+      <c r="G41" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="H41" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I41" s="9" t="s">
+      <c r="I41" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J41" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K41" s="9" t="s">
+      <c r="L41" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="M41" s="9"/>
+      <c r="N41" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="O41" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R41" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>101</v>
       </c>
@@ -4297,41 +4389,43 @@
       <c r="E42" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" s="1"/>
+      <c r="G42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="H42" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I42" s="9" t="s">
+      <c r="I42" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J42" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K42" s="9" t="s">
+      <c r="L42" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="L42" s="6" t="s">
+      <c r="M42" s="9"/>
+      <c r="N42" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="M42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="O42" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R42" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>103</v>
       </c>
@@ -4347,41 +4441,43 @@
       <c r="E43" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="1"/>
+      <c r="G43" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="H43" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="J43" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K43" s="9" t="s">
+      <c r="L43" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="M43" s="9"/>
+      <c r="N43" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="O43" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="N43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R43" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>106</v>
       </c>
@@ -4397,41 +4493,43 @@
       <c r="E44" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" s="1"/>
+      <c r="G44" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G44" s="9" t="s">
+      <c r="H44" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I44" s="9" t="s">
+      <c r="I44" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J44" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K44" s="9" t="s">
+      <c r="L44" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="M44" s="9"/>
+      <c r="N44" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="O44" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="N44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O44" s="6" t="s">
+      <c r="P44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q44" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="P44" s="1" t="s">
+      <c r="R44" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>109</v>
       </c>
@@ -4447,41 +4545,43 @@
       <c r="E45" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="1"/>
+      <c r="G45" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G45" s="9" t="s">
+      <c r="H45" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I45" s="9" t="s">
+      <c r="I45" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J45" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="K45" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K45" s="9" t="s">
+      <c r="L45" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="L45" s="1" t="s">
+      <c r="M45" s="9"/>
+      <c r="N45" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M45" s="1" t="s">
+      <c r="O45" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="N45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O45" s="6" t="s">
+      <c r="P45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q45" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="P45" s="1" t="s">
+      <c r="R45" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>110</v>
       </c>
@@ -4497,41 +4597,43 @@
       <c r="E46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F46" s="1"/>
+      <c r="G46" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="H46" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I46" s="9" t="s">
+      <c r="I46" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J46" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="K46" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K46" s="9" t="s">
+      <c r="L46" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="M46" s="9"/>
+      <c r="N46" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="O46" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="N46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O46" s="6" t="s">
+      <c r="P46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q46" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="P46" s="1" t="s">
+      <c r="R46" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>111</v>
       </c>
@@ -4547,41 +4649,43 @@
       <c r="E47" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="1"/>
+      <c r="G47" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="H47" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I47" s="9" t="s">
+      <c r="I47" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J47" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K47" s="9" t="s">
+      <c r="L47" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="M47" s="9"/>
+      <c r="N47" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="O47" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O47" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="P47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R47" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>113</v>
       </c>
@@ -4597,41 +4701,43 @@
       <c r="E48" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48" s="1"/>
+      <c r="G48" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="H48" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I48" s="9" t="s">
+      <c r="I48" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J48" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="K48" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K48" s="9" t="s">
+      <c r="L48" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="M48" s="9"/>
+      <c r="N48" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="M48" s="1" t="s">
+      <c r="O48" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O48" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R48" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>115</v>
       </c>
@@ -4647,41 +4753,43 @@
       <c r="E49" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F49" s="1"/>
+      <c r="G49" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="H49" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I49" s="9" t="s">
+      <c r="I49" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J49" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K49" s="9" t="s">
+      <c r="L49" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="L49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="M49" s="9"/>
       <c r="N49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P49" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="O49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P49" s="1" t="s">
+      <c r="Q49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R49" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>116</v>
       </c>
@@ -4697,41 +4805,43 @@
       <c r="E50" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" s="1"/>
+      <c r="G50" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="H50" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="H50" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I50" s="9" t="s">
+      <c r="I50" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J50" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K50" s="9" t="s">
+      <c r="L50" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="L50" s="1" t="s">
+      <c r="M50" s="9"/>
+      <c r="N50" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="M50" s="1" t="s">
+      <c r="O50" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O50" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="P50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q50" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R50" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>118</v>
       </c>
@@ -4747,41 +4857,43 @@
       <c r="E51" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51" s="1"/>
+      <c r="G51" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="H51" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I51" s="9" t="s">
+      <c r="I51" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J51" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J51" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K51" s="9" t="s">
+      <c r="L51" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="L51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="M51" s="9"/>
       <c r="N51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P51" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="O51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P51" s="1" t="s">
+      <c r="Q51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R51" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>119</v>
       </c>
@@ -4797,41 +4909,43 @@
       <c r="E52" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F52" s="1"/>
+      <c r="G52" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="H52" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I52" s="9" t="s">
+      <c r="I52" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J52" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="K52" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K52" s="9" t="s">
+      <c r="L52" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L52" s="7" t="s">
+      <c r="M52" s="9"/>
+      <c r="N52" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M52" s="1" t="s">
+      <c r="O52" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R52" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>122</v>
       </c>
@@ -4847,41 +4961,43 @@
       <c r="E53" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F53" s="1"/>
+      <c r="G53" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G53" s="9" t="s">
+      <c r="H53" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I53" s="9" t="s">
+      <c r="I53" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J53" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="K53" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K53" s="9" t="s">
+      <c r="L53" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L53" s="7" t="s">
+      <c r="M53" s="9"/>
+      <c r="N53" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M53" s="1" t="s">
+      <c r="O53" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O53" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R53" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>123</v>
       </c>
@@ -4897,41 +5013,43 @@
       <c r="E54" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" s="1"/>
+      <c r="G54" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G54" s="9" t="s">
+      <c r="H54" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="I54" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I54" s="8" t="s">
+      <c r="J54" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J54" s="1" t="s">
+      <c r="K54" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K54" s="9" t="s">
+      <c r="L54" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L54" s="7" t="s">
+      <c r="M54" s="9"/>
+      <c r="N54" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M54" s="1" t="s">
+      <c r="O54" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O54" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R54" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>127</v>
       </c>
@@ -4947,41 +5065,43 @@
       <c r="E55" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F55" s="1"/>
+      <c r="G55" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G55" s="9" t="s">
+      <c r="H55" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="I55" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I55" s="8" t="s">
+      <c r="J55" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J55" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K55" s="9" t="s">
+      <c r="L55" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L55" s="7" t="s">
+      <c r="M55" s="9"/>
+      <c r="N55" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M55" s="1" t="s">
+      <c r="O55" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O55" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R55" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>129</v>
       </c>
@@ -4997,41 +5117,43 @@
       <c r="E56" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F56" s="1"/>
+      <c r="G56" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="H56" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="I56" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I56" s="8" t="s">
+      <c r="J56" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J56" s="1" t="s">
+      <c r="K56" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K56" s="9" t="s">
+      <c r="L56" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L56" s="7" t="s">
+      <c r="M56" s="9"/>
+      <c r="N56" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M56" s="1" t="s">
+      <c r="O56" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O56" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R56" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>131</v>
       </c>
@@ -5047,41 +5169,43 @@
       <c r="E57" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F57" s="1"/>
+      <c r="G57" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G57" s="9" t="s">
+      <c r="H57" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I57" s="8" t="s">
+      <c r="J57" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J57" s="1" t="s">
+      <c r="K57" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K57" s="9" t="s">
+      <c r="L57" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L57" s="7" t="s">
+      <c r="M57" s="9"/>
+      <c r="N57" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M57" s="1" t="s">
+      <c r="O57" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O57" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R57" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>133</v>
       </c>
@@ -5097,41 +5221,43 @@
       <c r="E58" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" s="1"/>
+      <c r="G58" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G58" s="9" t="s">
+      <c r="H58" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="H58" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I58" s="9" t="s">
+      <c r="I58" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J58" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J58" s="1" t="s">
+      <c r="K58" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K58" s="9" t="s">
+      <c r="L58" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L58" s="7" t="s">
+      <c r="M58" s="9"/>
+      <c r="N58" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M58" s="1" t="s">
+      <c r="O58" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O58" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R58" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>134</v>
       </c>
@@ -5147,41 +5273,43 @@
       <c r="E59" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F59" s="1"/>
+      <c r="G59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G59" s="9" t="s">
+      <c r="H59" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="H59" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I59" s="9" t="s">
+      <c r="I59" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J59" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J59" s="1" t="s">
+      <c r="K59" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K59" s="9" t="s">
+      <c r="L59" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L59" s="7" t="s">
+      <c r="M59" s="9"/>
+      <c r="N59" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M59" s="1" t="s">
+      <c r="O59" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N59" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O59" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R59" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>135</v>
       </c>
@@ -5197,41 +5325,43 @@
       <c r="E60" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F60" s="1"/>
+      <c r="G60" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G60" s="9" t="s">
+      <c r="H60" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I60" s="9" t="s">
+      <c r="I60" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J60" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J60" s="1" t="s">
+      <c r="K60" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K60" s="9" t="s">
+      <c r="L60" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L60" s="7" t="s">
+      <c r="M60" s="9"/>
+      <c r="N60" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M60" s="1" t="s">
+      <c r="O60" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N60" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R60" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>136</v>
       </c>
@@ -5247,41 +5377,43 @@
       <c r="E61" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F61" s="1"/>
+      <c r="G61" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G61" s="9" t="s">
+      <c r="H61" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="H61" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I61" s="9" t="s">
+      <c r="I61" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J61" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J61" s="1" t="s">
+      <c r="K61" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K61" s="9" t="s">
+      <c r="L61" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L61" s="7" t="s">
+      <c r="M61" s="9"/>
+      <c r="N61" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M61" s="1" t="s">
+      <c r="O61" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O61" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R61" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>137</v>
       </c>
@@ -5297,41 +5429,43 @@
       <c r="E62" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F62" s="1"/>
+      <c r="G62" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G62" s="9" t="s">
+      <c r="H62" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="I62" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I62" s="8" t="s">
+      <c r="J62" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J62" s="1" t="s">
+      <c r="K62" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="K62" s="9" t="s">
+      <c r="L62" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="L62" s="7" t="s">
+      <c r="M62" s="9"/>
+      <c r="N62" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M62" s="1" t="s">
+      <c r="O62" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N62" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O62" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R62" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>139</v>
       </c>
@@ -5347,41 +5481,43 @@
       <c r="E63" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" s="1"/>
+      <c r="G63" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G63" s="9" t="s">
+      <c r="H63" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I63" s="9" t="s">
+      <c r="I63" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J63" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J63" s="1" t="s">
+      <c r="K63" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="K63" s="9" t="s">
+      <c r="L63" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="L63" s="7" t="s">
+      <c r="M63" s="9"/>
+      <c r="N63" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M63" s="1" t="s">
+      <c r="O63" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N63" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O63" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R63" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>141</v>
       </c>
@@ -5397,41 +5533,43 @@
       <c r="E64" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" s="1"/>
+      <c r="G64" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G64" s="9" t="s">
+      <c r="H64" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I64" s="9" t="s">
+      <c r="I64" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J64" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J64" s="1" t="s">
+      <c r="K64" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="K64" s="9" t="s">
+      <c r="L64" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="L64" s="7" t="s">
+      <c r="M64" s="9"/>
+      <c r="N64" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M64" s="1" t="s">
+      <c r="O64" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N64" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O64" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R64" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>142</v>
       </c>
@@ -5447,41 +5585,43 @@
       <c r="E65" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F65" s="1"/>
+      <c r="G65" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G65" s="9" t="s">
+      <c r="H65" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="H65" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I65" s="9" t="s">
+      <c r="I65" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J65" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J65" s="1" t="s">
+      <c r="K65" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="K65" s="9" t="s">
+      <c r="L65" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="L65" s="7" t="s">
+      <c r="M65" s="9"/>
+      <c r="N65" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M65" s="1" t="s">
+      <c r="O65" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N65" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O65" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R65" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>143</v>
       </c>
@@ -5497,41 +5637,43 @@
       <c r="E66" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F66" s="1"/>
+      <c r="G66" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G66" s="9" t="s">
+      <c r="H66" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="H66" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I66" s="9" t="s">
+      <c r="I66" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J66" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J66" s="1" t="s">
+      <c r="K66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K66" s="9" t="s">
+      <c r="L66" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="L66" s="1" t="s">
+      <c r="M66" s="9"/>
+      <c r="N66" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="M66" s="1" t="s">
+      <c r="O66" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N66" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O66" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R66" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>145</v>
       </c>
@@ -5547,41 +5689,43 @@
       <c r="E67" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="F67" s="1"/>
+      <c r="G67" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G67" s="9" t="s">
+      <c r="H67" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="H67" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I67" s="9" t="s">
+      <c r="I67" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J67" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J67" s="1" t="s">
+      <c r="K67" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K67" s="9" t="s">
+      <c r="L67" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="L67" s="1" t="s">
+      <c r="M67" s="9"/>
+      <c r="N67" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="M67" s="1" t="s">
+      <c r="O67" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N67" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O67" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R67" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>147</v>
       </c>
@@ -5597,41 +5741,43 @@
       <c r="E68" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F68" s="1"/>
+      <c r="G68" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G68" s="9" t="s">
+      <c r="H68" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="H68" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I68" s="9" t="s">
+      <c r="I68" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J68" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J68" s="1" t="s">
+      <c r="K68" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="K68" s="9" t="s">
+      <c r="L68" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="L68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M68" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="M68" s="9"/>
       <c r="N68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P68" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="O68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P68" s="1" t="s">
+      <c r="Q68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R68" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>149</v>
       </c>
@@ -5647,41 +5793,43 @@
       <c r="E69" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F69" s="1"/>
+      <c r="G69" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G69" s="9" t="s">
+      <c r="H69" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="I69" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I69" s="8" t="s">
+      <c r="J69" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J69" s="1" t="s">
+      <c r="K69" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="K69" s="9" t="s">
+      <c r="L69" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="L69" s="7" t="s">
+      <c r="M69" s="9"/>
+      <c r="N69" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M69" s="1" t="s">
+      <c r="O69" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N69" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O69" s="1" t="s">
+      <c r="P69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q69" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="P69" s="1" t="s">
+      <c r="R69" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>153</v>
       </c>
@@ -5697,41 +5845,43 @@
       <c r="E70" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F70" s="1"/>
+      <c r="G70" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G70" s="9" t="s">
+      <c r="H70" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="I70" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I70" s="8" t="s">
+      <c r="J70" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J70" s="1" t="s">
+      <c r="K70" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="K70" s="9" t="s">
+      <c r="L70" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="L70" s="7" t="s">
+      <c r="M70" s="9"/>
+      <c r="N70" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M70" s="1" t="s">
+      <c r="O70" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N70" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O70" s="1" t="s">
+      <c r="P70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q70" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="P70" s="1" t="s">
+      <c r="R70" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>154</v>
       </c>
@@ -5747,41 +5897,43 @@
       <c r="E71" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="F71" s="1"/>
+      <c r="G71" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G71" s="9" t="s">
+      <c r="H71" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="H71" s="1" t="s">
+      <c r="I71" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I71" s="8" t="s">
+      <c r="J71" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J71" s="1" t="s">
+      <c r="K71" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K71" s="9" t="s">
+      <c r="L71" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L71" s="7" t="s">
+      <c r="M71" s="9"/>
+      <c r="N71" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M71" s="1" t="s">
+      <c r="O71" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N71" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O71" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R71" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>158</v>
       </c>
@@ -5797,41 +5949,43 @@
       <c r="E72" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="F72" s="1"/>
+      <c r="G72" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G72" s="9" t="s">
+      <c r="H72" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="H72" s="1" t="s">
+      <c r="I72" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I72" s="8" t="s">
+      <c r="J72" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J72" s="1" t="s">
+      <c r="K72" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K72" s="9" t="s">
+      <c r="L72" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L72" s="7" t="s">
+      <c r="M72" s="9"/>
+      <c r="N72" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M72" s="1" t="s">
+      <c r="O72" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N72" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O72" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P72" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q72" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R72" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>160</v>
       </c>
@@ -5847,41 +6001,43 @@
       <c r="E73" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F73" s="1"/>
+      <c r="G73" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G73" s="9" t="s">
+      <c r="H73" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="H73" s="1" t="s">
+      <c r="I73" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I73" s="8" t="s">
+      <c r="J73" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J73" s="1" t="s">
+      <c r="K73" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K73" s="9" t="s">
+      <c r="L73" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L73" s="7" t="s">
+      <c r="M73" s="9"/>
+      <c r="N73" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M73" s="1" t="s">
+      <c r="O73" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N73" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O73" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R73" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>162</v>
       </c>
@@ -5897,41 +6053,43 @@
       <c r="E74" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F74" s="1"/>
+      <c r="G74" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G74" s="9" t="s">
+      <c r="H74" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="H74" s="1" t="s">
+      <c r="I74" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I74" s="8" t="s">
+      <c r="J74" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="J74" s="1" t="s">
+      <c r="K74" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="K74" s="9" t="s">
+      <c r="L74" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="L74" s="7" t="s">
+      <c r="M74" s="9"/>
+      <c r="N74" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M74" s="1" t="s">
+      <c r="O74" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N74" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O74" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R74" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>164</v>
       </c>
@@ -5947,41 +6105,43 @@
       <c r="E75" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F75" s="1" t="s">
+      <c r="F75" s="1"/>
+      <c r="G75" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G75" s="9" t="s">
+      <c r="H75" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="H75" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I75" s="9" t="s">
+      <c r="I75" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J75" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J75" s="1" t="s">
+      <c r="K75" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K75" s="9" t="s">
+      <c r="L75" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="L75" s="1" t="s">
+      <c r="M75" s="9"/>
+      <c r="N75" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M75" s="1" t="s">
+      <c r="O75" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="N75" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O75" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R75" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>166</v>
       </c>
@@ -5997,41 +6157,43 @@
       <c r="E76" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="F76" s="1"/>
+      <c r="G76" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G76" s="9" t="s">
+      <c r="H76" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="H76" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I76" s="9" t="s">
+      <c r="I76" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J76" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J76" s="1" t="s">
+      <c r="K76" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K76" s="9" t="s">
+      <c r="L76" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="L76" s="1" t="s">
+      <c r="M76" s="9"/>
+      <c r="N76" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M76" s="1" t="s">
+      <c r="O76" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="N76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O76" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R76" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>167</v>
       </c>
@@ -6047,42 +6209,44 @@
       <c r="E77" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F77" s="1"/>
+      <c r="G77" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G77" s="9" t="s">
+      <c r="H77" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="H77" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I77" s="9" t="s">
+      <c r="I77" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J77" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="J77" s="1" t="s">
+      <c r="K77" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K77" s="9" t="s">
+      <c r="L77" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="L77" s="1" t="s">
+      <c r="M77" s="9"/>
+      <c r="N77" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M77" s="1" t="s">
+      <c r="O77" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="N77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O77" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="P77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R77" s="1" t="s">
         <v>218</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:P78">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R78">
     <sortCondition ref="A2:A78"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
19tto20T targets populate new pe column
</commit_message>
<xml_diff>
--- a/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
+++ b/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/site_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{36FB4EA7-CA82-E348-989B-9500E8620989}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3D6F20AC-ADC3-1E45-B210-BFADB3E73B5C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1674" uniqueCount="437">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1750" uniqueCount="438">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -1344,6 +1344,9 @@
   </si>
   <si>
     <t>DE_GROUP-zhdJiWlPvCz</t>
+  </si>
+  <si>
+    <t>2018Oct</t>
   </si>
 </sst>
 </file>
@@ -2217,9 +2220,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2336,7 +2337,9 @@
       <c r="L2" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="M2" s="4"/>
+      <c r="M2" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N2" s="4" t="s">
         <v>9</v>
       </c>
@@ -2390,7 +2393,9 @@
       <c r="L3" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="M3" s="4"/>
+      <c r="M3" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N3" s="4" t="s">
         <v>9</v>
       </c>
@@ -2444,7 +2449,9 @@
       <c r="L4" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="M4" s="4"/>
+      <c r="M4" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N4" s="4" t="s">
         <v>213</v>
       </c>
@@ -2498,7 +2505,9 @@
       <c r="L5" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="M5" s="4"/>
+      <c r="M5" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N5" s="4" t="s">
         <v>213</v>
       </c>
@@ -2552,7 +2561,9 @@
       <c r="L6" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="M6" s="4"/>
+      <c r="M6" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N6" s="4" t="s">
         <v>213</v>
       </c>
@@ -2606,7 +2617,9 @@
       <c r="L7" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="M7" s="4"/>
+      <c r="M7" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N7" s="4" t="s">
         <v>213</v>
       </c>
@@ -2660,7 +2673,9 @@
       <c r="L8" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="M8" s="4"/>
+      <c r="M8" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N8" s="4" t="s">
         <v>211</v>
       </c>
@@ -2714,7 +2729,9 @@
       <c r="L9" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="M9" s="4"/>
+      <c r="M9" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N9" s="4" t="s">
         <v>211</v>
       </c>
@@ -2768,7 +2785,9 @@
       <c r="L10" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N10" s="4" t="s">
         <v>213</v>
       </c>
@@ -2822,7 +2841,9 @@
       <c r="L11" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N11" s="4" t="s">
         <v>213</v>
       </c>
@@ -2876,7 +2897,9 @@
       <c r="L12" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="M12" s="4"/>
+      <c r="M12" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N12" s="4" t="s">
         <v>213</v>
       </c>
@@ -2930,7 +2953,9 @@
       <c r="L13" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="M13" s="4"/>
+      <c r="M13" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N13" s="4" t="s">
         <v>213</v>
       </c>
@@ -2984,7 +3009,9 @@
       <c r="L14" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="M14" s="4"/>
+      <c r="M14" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N14" s="4" t="s">
         <v>215</v>
       </c>
@@ -3038,7 +3065,9 @@
       <c r="L15" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="M15" s="4"/>
+      <c r="M15" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N15" s="4" t="s">
         <v>215</v>
       </c>
@@ -3092,7 +3121,9 @@
       <c r="L16" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="M16" s="4"/>
+      <c r="M16" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N16" s="4" t="s">
         <v>213</v>
       </c>
@@ -3146,7 +3177,9 @@
       <c r="L17" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="M17" s="4"/>
+      <c r="M17" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N17" s="4" t="s">
         <v>213</v>
       </c>
@@ -3200,7 +3233,9 @@
       <c r="L18" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="M18" s="4"/>
+      <c r="M18" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N18" s="4" t="s">
         <v>213</v>
       </c>
@@ -3254,7 +3289,9 @@
       <c r="L19" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="M19" s="4"/>
+      <c r="M19" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N19" s="4" t="s">
         <v>213</v>
       </c>
@@ -3308,7 +3345,9 @@
       <c r="L20" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="M20" s="4"/>
+      <c r="M20" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N20" s="4" t="s">
         <v>213</v>
       </c>
@@ -3362,7 +3401,9 @@
       <c r="L21" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="M21" s="4"/>
+      <c r="M21" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N21" s="4" t="s">
         <v>213</v>
       </c>
@@ -3416,7 +3457,9 @@
       <c r="L22" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="M22" s="4"/>
+      <c r="M22" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N22" s="4" t="s">
         <v>215</v>
       </c>
@@ -3470,7 +3513,9 @@
       <c r="L23" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="M23" s="4"/>
+      <c r="M23" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N23" s="4" t="s">
         <v>215</v>
       </c>
@@ -3524,7 +3569,9 @@
       <c r="L24" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="M24" s="4"/>
+      <c r="M24" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N24" s="4" t="s">
         <v>213</v>
       </c>
@@ -3578,7 +3625,9 @@
       <c r="L25" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="M25" s="4"/>
+      <c r="M25" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N25" s="4" t="s">
         <v>213</v>
       </c>
@@ -3632,7 +3681,9 @@
       <c r="L26" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="M26" s="4"/>
+      <c r="M26" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N26" s="4" t="s">
         <v>213</v>
       </c>
@@ -3686,7 +3737,9 @@
       <c r="L27" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="M27" s="4"/>
+      <c r="M27" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N27" s="4" t="s">
         <v>213</v>
       </c>
@@ -3740,7 +3793,9 @@
       <c r="L28" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="M28" s="4"/>
+      <c r="M28" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N28" s="4" t="s">
         <v>213</v>
       </c>
@@ -3794,7 +3849,9 @@
       <c r="L29" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="M29" s="4"/>
+      <c r="M29" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N29" s="4" t="s">
         <v>213</v>
       </c>
@@ -3848,7 +3905,9 @@
       <c r="L30" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="M30" s="4"/>
+      <c r="M30" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N30" s="4" t="s">
         <v>213</v>
       </c>
@@ -3902,7 +3961,9 @@
       <c r="L31" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="M31" s="4"/>
+      <c r="M31" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N31" s="4" t="s">
         <v>213</v>
       </c>
@@ -3956,7 +4017,9 @@
       <c r="L32" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="M32" s="4"/>
+      <c r="M32" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N32" s="4" t="s">
         <v>9</v>
       </c>
@@ -4010,7 +4073,9 @@
       <c r="L33" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="M33" s="4"/>
+      <c r="M33" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N33" s="4" t="s">
         <v>9</v>
       </c>
@@ -4064,7 +4129,9 @@
       <c r="L34" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="M34" s="4"/>
+      <c r="M34" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N34" s="4" t="s">
         <v>9</v>
       </c>
@@ -4118,7 +4185,9 @@
       <c r="L35" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="M35" s="4"/>
+      <c r="M35" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N35" s="4" t="s">
         <v>9</v>
       </c>
@@ -4172,7 +4241,9 @@
       <c r="L36" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="M36" s="4"/>
+      <c r="M36" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N36" s="4" t="s">
         <v>9</v>
       </c>
@@ -4226,7 +4297,9 @@
       <c r="L37" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="M37" s="4"/>
+      <c r="M37" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N37" s="4" t="s">
         <v>353</v>
       </c>
@@ -4280,7 +4353,9 @@
       <c r="L38" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="M38" s="4"/>
+      <c r="M38" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N38" s="4" t="s">
         <v>353</v>
       </c>
@@ -4334,7 +4409,9 @@
       <c r="L39" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="M39" s="4"/>
+      <c r="M39" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N39" s="4" t="s">
         <v>9</v>
       </c>
@@ -4388,7 +4465,9 @@
       <c r="L40" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="M40" s="4"/>
+      <c r="M40" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N40" s="4" t="s">
         <v>9</v>
       </c>
@@ -4442,7 +4521,9 @@
       <c r="L41" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="M41" s="4"/>
+      <c r="M41" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N41" s="4" t="s">
         <v>221</v>
       </c>
@@ -4496,7 +4577,9 @@
       <c r="L42" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="M42" s="4"/>
+      <c r="M42" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N42" s="4" t="s">
         <v>222</v>
       </c>
@@ -4550,7 +4633,9 @@
       <c r="L43" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="M43" s="4"/>
+      <c r="M43" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N43" s="4" t="s">
         <v>211</v>
       </c>
@@ -4604,7 +4689,9 @@
       <c r="L44" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="M44" s="4"/>
+      <c r="M44" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N44" s="4" t="s">
         <v>211</v>
       </c>
@@ -4658,7 +4745,9 @@
       <c r="L45" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="M45" s="4"/>
+      <c r="M45" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N45" s="4" t="s">
         <v>211</v>
       </c>
@@ -4712,7 +4801,9 @@
       <c r="L46" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="M46" s="4"/>
+      <c r="M46" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N46" s="4" t="s">
         <v>211</v>
       </c>
@@ -4766,7 +4857,9 @@
       <c r="L47" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="M47" s="4"/>
+      <c r="M47" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N47" s="4" t="s">
         <v>211</v>
       </c>
@@ -4820,7 +4913,9 @@
       <c r="L48" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="M48" s="4"/>
+      <c r="M48" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N48" s="4" t="s">
         <v>224</v>
       </c>
@@ -4874,7 +4969,9 @@
       <c r="L49" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="M49" s="4"/>
+      <c r="M49" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N49" s="4" t="s">
         <v>9</v>
       </c>
@@ -4928,7 +5025,9 @@
       <c r="L50" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="M50" s="4"/>
+      <c r="M50" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N50" s="4" t="s">
         <v>224</v>
       </c>
@@ -4982,7 +5081,9 @@
       <c r="L51" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="M51" s="4"/>
+      <c r="M51" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N51" s="4" t="s">
         <v>9</v>
       </c>
@@ -5036,7 +5137,9 @@
       <c r="L52" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M52" s="4"/>
+      <c r="M52" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N52" s="4" t="s">
         <v>360</v>
       </c>
@@ -5090,7 +5193,9 @@
       <c r="L53" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M53" s="4"/>
+      <c r="M53" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N53" s="4" t="s">
         <v>360</v>
       </c>
@@ -5144,7 +5249,9 @@
       <c r="L54" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M54" s="4"/>
+      <c r="M54" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N54" s="4" t="s">
         <v>360</v>
       </c>
@@ -5198,7 +5305,9 @@
       <c r="L55" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M55" s="4"/>
+      <c r="M55" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N55" s="4" t="s">
         <v>360</v>
       </c>
@@ -5252,7 +5361,9 @@
       <c r="L56" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M56" s="4"/>
+      <c r="M56" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N56" s="4" t="s">
         <v>360</v>
       </c>
@@ -5306,7 +5417,9 @@
       <c r="L57" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M57" s="4"/>
+      <c r="M57" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N57" s="4" t="s">
         <v>360</v>
       </c>
@@ -5360,7 +5473,9 @@
       <c r="L58" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M58" s="4"/>
+      <c r="M58" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N58" s="4" t="s">
         <v>360</v>
       </c>
@@ -5414,7 +5529,9 @@
       <c r="L59" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M59" s="4"/>
+      <c r="M59" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N59" s="4" t="s">
         <v>360</v>
       </c>
@@ -5468,7 +5585,9 @@
       <c r="L60" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M60" s="4"/>
+      <c r="M60" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N60" s="4" t="s">
         <v>360</v>
       </c>
@@ -5522,7 +5641,9 @@
       <c r="L61" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M61" s="4"/>
+      <c r="M61" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N61" s="4" t="s">
         <v>360</v>
       </c>
@@ -5576,7 +5697,9 @@
       <c r="L62" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="M62" s="4"/>
+      <c r="M62" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N62" s="4" t="s">
         <v>360</v>
       </c>
@@ -5630,7 +5753,9 @@
       <c r="L63" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="M63" s="4"/>
+      <c r="M63" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N63" s="4" t="s">
         <v>360</v>
       </c>
@@ -5684,7 +5809,9 @@
       <c r="L64" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="M64" s="4"/>
+      <c r="M64" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N64" s="4" t="s">
         <v>360</v>
       </c>
@@ -5738,7 +5865,9 @@
       <c r="L65" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="M65" s="4"/>
+      <c r="M65" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N65" s="4" t="s">
         <v>360</v>
       </c>
@@ -5792,7 +5921,9 @@
       <c r="L66" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="M66" s="4"/>
+      <c r="M66" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N66" s="4" t="s">
         <v>361</v>
       </c>
@@ -5846,7 +5977,9 @@
       <c r="L67" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="M67" s="4"/>
+      <c r="M67" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N67" s="4" t="s">
         <v>361</v>
       </c>
@@ -5900,7 +6033,9 @@
       <c r="L68" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="M68" s="4"/>
+      <c r="M68" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N68" s="4" t="s">
         <v>9</v>
       </c>
@@ -5954,7 +6089,9 @@
       <c r="L69" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="M69" s="4"/>
+      <c r="M69" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N69" s="4" t="s">
         <v>360</v>
       </c>
@@ -6008,7 +6145,9 @@
       <c r="L70" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="M70" s="4"/>
+      <c r="M70" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N70" s="4" t="s">
         <v>360</v>
       </c>
@@ -6062,7 +6201,9 @@
       <c r="L71" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M71" s="4"/>
+      <c r="M71" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N71" s="4" t="s">
         <v>360</v>
       </c>
@@ -6116,7 +6257,9 @@
       <c r="L72" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M72" s="4"/>
+      <c r="M72" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N72" s="4" t="s">
         <v>360</v>
       </c>
@@ -6170,7 +6313,9 @@
       <c r="L73" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M73" s="4"/>
+      <c r="M73" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N73" s="4" t="s">
         <v>360</v>
       </c>
@@ -6224,7 +6369,9 @@
       <c r="L74" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="M74" s="4"/>
+      <c r="M74" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N74" s="4" t="s">
         <v>360</v>
       </c>
@@ -6278,7 +6425,9 @@
       <c r="L75" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="M75" s="4"/>
+      <c r="M75" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N75" s="4" t="s">
         <v>211</v>
       </c>
@@ -6332,7 +6481,9 @@
       <c r="L76" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="M76" s="4"/>
+      <c r="M76" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N76" s="4" t="s">
         <v>211</v>
       </c>
@@ -6386,7 +6537,9 @@
       <c r="L77" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="M77" s="4"/>
+      <c r="M77" s="4" t="s">
+        <v>437</v>
+      </c>
       <c r="N77" s="4" t="s">
         <v>211</v>
       </c>

</xml_diff>

<commit_message>
dim_Item_sets_config file add dim_cop_type_site column with elements to match datapack input and expected output column names
</commit_message>
<xml_diff>
--- a/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
+++ b/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/site_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3D6F20AC-ADC3-1E45-B210-BFADB3E73B5C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1C5AAE1B-B992-FB4D-AD39-12915A40FA0B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1750" uniqueCount="438">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1750" uniqueCount="441">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -1169,9 +1169,6 @@
     <t>Other_fy20_cop</t>
   </si>
   <si>
-    <t>other_disagg</t>
-  </si>
-  <si>
     <t>disagg_type</t>
   </si>
   <si>
@@ -1347,6 +1344,18 @@
   </si>
   <si>
     <t>2018Oct</t>
+  </si>
+  <si>
+    <t>Age_set</t>
+  </si>
+  <si>
+    <t>Sex_set</t>
+  </si>
+  <si>
+    <t>KeyPop_set</t>
+  </si>
+  <si>
+    <t>OtherDisagg_set</t>
   </si>
 </sst>
 </file>
@@ -2220,7 +2229,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2238,9 +2249,9 @@
     <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2255,46 +2266,46 @@
         <v>376</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>377</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>204</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>205</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>383</v>
-      </c>
       <c r="M1" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>207</v>
+        <v>437</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>208</v>
+        <v>438</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>209</v>
+        <v>439</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>378</v>
+        <v>440</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>217</v>
@@ -2317,28 +2328,28 @@
         <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>9</v>
@@ -2373,28 +2384,28 @@
         <v>15</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>9</v>
@@ -2429,28 +2440,28 @@
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>196</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>213</v>
@@ -2485,28 +2496,28 @@
         <v>21</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>196</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>213</v>
@@ -2541,28 +2552,28 @@
         <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>182</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>213</v>
@@ -2597,28 +2608,28 @@
         <v>21</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>182</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>213</v>
@@ -2653,28 +2664,28 @@
         <v>33</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>211</v>
@@ -2709,28 +2720,28 @@
         <v>36</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>32</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>211</v>
@@ -2765,28 +2776,28 @@
         <v>39</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>186</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>213</v>
@@ -2821,28 +2832,28 @@
         <v>41</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>186</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>213</v>
@@ -2877,28 +2888,28 @@
         <v>39</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>199</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>213</v>
@@ -2933,28 +2944,28 @@
         <v>41</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>199</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>213</v>
@@ -2989,28 +3000,28 @@
         <v>39</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>197</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>215</v>
@@ -3045,28 +3056,28 @@
         <v>41</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>197</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>215</v>
@@ -3101,28 +3112,28 @@
         <v>39</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>177</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>213</v>
@@ -3157,28 +3168,28 @@
         <v>41</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>177</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>213</v>
@@ -3213,28 +3224,28 @@
         <v>39</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>193</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>213</v>
@@ -3269,28 +3280,28 @@
         <v>41</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>193</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>213</v>
@@ -3325,28 +3336,28 @@
         <v>39</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>179</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>213</v>
@@ -3381,28 +3392,28 @@
         <v>41</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>179</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>213</v>
@@ -3437,28 +3448,28 @@
         <v>39</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>190</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>215</v>
@@ -3493,28 +3504,28 @@
         <v>41</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>190</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>215</v>
@@ -3549,28 +3560,28 @@
         <v>39</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>194</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>213</v>
@@ -3605,28 +3616,28 @@
         <v>41</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>194</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>213</v>
@@ -3661,28 +3672,28 @@
         <v>39</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>188</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>213</v>
@@ -3717,28 +3728,28 @@
         <v>41</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>188</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>213</v>
@@ -3773,28 +3784,28 @@
         <v>39</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>202</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>213</v>
@@ -3829,28 +3840,28 @@
         <v>41</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>202</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>213</v>
@@ -3885,28 +3896,28 @@
         <v>39</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>183</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>213</v>
@@ -3941,28 +3952,28 @@
         <v>41</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>183</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>213</v>
@@ -3997,28 +4008,28 @@
         <v>39</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>74</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>9</v>
@@ -4053,28 +4064,28 @@
         <v>41</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>74</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>9</v>
@@ -4109,28 +4120,28 @@
         <v>9</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>78</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>9</v>
@@ -4165,28 +4176,28 @@
         <v>9</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>80</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>81</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>9</v>
@@ -4221,28 +4232,28 @@
         <v>9</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>181</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>9</v>
@@ -4277,28 +4288,28 @@
         <v>88</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>86</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>353</v>
@@ -4333,28 +4344,28 @@
         <v>90</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>86</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>353</v>
@@ -4389,28 +4400,28 @@
         <v>94</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>92</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>203</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>9</v>
@@ -4445,28 +4456,28 @@
         <v>96</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>92</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>203</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>9</v>
@@ -4501,28 +4512,28 @@
         <v>100</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>99</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>221</v>
@@ -4557,28 +4568,28 @@
         <v>102</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I42" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>99</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>222</v>
@@ -4613,28 +4624,28 @@
         <v>9</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>104</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>211</v>
@@ -4669,28 +4680,28 @@
         <v>108</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>104</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>107</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>211</v>
@@ -4725,28 +4736,28 @@
         <v>19</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>104</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>107</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>211</v>
@@ -4781,28 +4792,28 @@
         <v>21</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>104</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K46" s="4" t="s">
         <v>107</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>211</v>
@@ -4837,28 +4848,28 @@
         <v>9</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>112</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K47" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>211</v>
@@ -4893,28 +4904,28 @@
         <v>9</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>117</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I48" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K48" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>224</v>
@@ -4949,28 +4960,28 @@
         <v>9</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>117</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K49" s="4" t="s">
         <v>81</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>9</v>
@@ -5005,28 +5016,28 @@
         <v>9</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>117</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I50" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K50" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>224</v>
@@ -5061,28 +5072,28 @@
         <v>9</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>117</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I51" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>81</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>9</v>
@@ -5117,28 +5128,28 @@
         <v>94</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>120</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I52" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K52" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>360</v>
@@ -5173,28 +5184,28 @@
         <v>96</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>120</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I53" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K53" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>360</v>
@@ -5229,28 +5240,28 @@
         <v>126</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K54" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>360</v>
@@ -5285,28 +5296,28 @@
         <v>128</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I55" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K55" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>360</v>
@@ -5341,28 +5352,28 @@
         <v>130</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I56" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K56" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>360</v>
@@ -5397,28 +5408,28 @@
         <v>132</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>360</v>
@@ -5453,28 +5464,28 @@
         <v>126</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K58" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N58" s="4" t="s">
         <v>360</v>
@@ -5509,28 +5520,28 @@
         <v>128</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I59" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K59" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N59" s="4" t="s">
         <v>360</v>
@@ -5565,28 +5576,28 @@
         <v>130</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I60" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K60" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N60" s="4" t="s">
         <v>360</v>
@@ -5621,28 +5632,28 @@
         <v>132</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K61" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N61" s="4" t="s">
         <v>360</v>
@@ -5677,28 +5688,28 @@
         <v>9</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>138</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I62" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K62" s="4" t="s">
         <v>176</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N62" s="4" t="s">
         <v>360</v>
@@ -5733,28 +5744,28 @@
         <v>108</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>138</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I63" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K63" s="4" t="s">
         <v>176</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>360</v>
@@ -5789,28 +5800,28 @@
         <v>19</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>138</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I64" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K64" s="4" t="s">
         <v>176</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>360</v>
@@ -5845,28 +5856,28 @@
         <v>21</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>138</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K65" s="4" t="s">
         <v>176</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N65" s="4" t="s">
         <v>360</v>
@@ -5901,28 +5912,28 @@
         <v>9</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>144</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I66" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K66" s="4" t="s">
         <v>8</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N66" s="4" t="s">
         <v>361</v>
@@ -5957,28 +5968,28 @@
         <v>9</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I67" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K67" s="4" t="s">
         <v>8</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N67" s="4" t="s">
         <v>361</v>
@@ -6013,28 +6024,28 @@
         <v>9</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I68" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K68" s="4" t="s">
         <v>148</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="M68" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N68" s="4" t="s">
         <v>9</v>
@@ -6069,28 +6080,28 @@
         <v>152</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>150</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I69" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K69" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N69" s="4" t="s">
         <v>360</v>
@@ -6125,28 +6136,28 @@
         <v>152</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>150</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I70" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K70" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N70" s="4" t="s">
         <v>360</v>
@@ -6181,28 +6192,28 @@
         <v>157</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>155</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I71" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K71" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N71" s="4" t="s">
         <v>360</v>
@@ -6237,28 +6248,28 @@
         <v>159</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>155</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I72" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K72" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N72" s="4" t="s">
         <v>360</v>
@@ -6293,28 +6304,28 @@
         <v>161</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>155</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I73" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K73" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N73" s="4" t="s">
         <v>360</v>
@@ -6349,28 +6360,28 @@
         <v>163</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>155</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I74" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K74" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N74" s="4" t="s">
         <v>360</v>
@@ -6405,28 +6416,28 @@
         <v>39</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>165</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I75" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K75" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N75" s="4" t="s">
         <v>211</v>
@@ -6461,28 +6472,28 @@
         <v>41</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>165</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K76" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N76" s="4" t="s">
         <v>211</v>
@@ -6517,28 +6528,28 @@
         <v>168</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>165</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I77" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K77" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N77" s="4" t="s">
         <v>211</v>

</xml_diff>

<commit_message>
Revert "dim_Item_sets_config file add dim_cop_type_site column with elements to match datapack input and expected output column names"
This reverts commit 0800fc00c35f595f1a2f979f0c152e8949db2ccd.
</commit_message>
<xml_diff>
--- a/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
+++ b/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/site_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1C5AAE1B-B992-FB4D-AD39-12915A40FA0B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3D6F20AC-ADC3-1E45-B210-BFADB3E73B5C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1750" uniqueCount="441">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1750" uniqueCount="438">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -1169,6 +1169,9 @@
     <t>Other_fy20_cop</t>
   </si>
   <si>
+    <t>other_disagg</t>
+  </si>
+  <si>
     <t>disagg_type</t>
   </si>
   <si>
@@ -1344,18 +1347,6 @@
   </si>
   <si>
     <t>2018Oct</t>
-  </si>
-  <si>
-    <t>Age_set</t>
-  </si>
-  <si>
-    <t>Sex_set</t>
-  </si>
-  <si>
-    <t>KeyPop_set</t>
-  </si>
-  <si>
-    <t>OtherDisagg_set</t>
   </si>
 </sst>
 </file>
@@ -2229,9 +2220,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2249,9 +2238,9 @@
     <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2266,46 +2255,46 @@
         <v>376</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>377</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>204</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>205</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>378</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>440</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>217</v>
@@ -2328,28 +2317,28 @@
         <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>9</v>
@@ -2384,28 +2373,28 @@
         <v>15</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>9</v>
@@ -2440,28 +2429,28 @@
         <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>196</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>213</v>
@@ -2496,28 +2485,28 @@
         <v>21</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>196</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>213</v>
@@ -2552,28 +2541,28 @@
         <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>182</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>213</v>
@@ -2608,28 +2597,28 @@
         <v>21</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>182</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>213</v>
@@ -2664,28 +2653,28 @@
         <v>33</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>211</v>
@@ -2720,28 +2709,28 @@
         <v>36</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>32</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>211</v>
@@ -2776,28 +2765,28 @@
         <v>39</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>186</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>213</v>
@@ -2832,28 +2821,28 @@
         <v>41</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>186</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>213</v>
@@ -2888,28 +2877,28 @@
         <v>39</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>199</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>213</v>
@@ -2944,28 +2933,28 @@
         <v>41</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>199</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>213</v>
@@ -3000,28 +2989,28 @@
         <v>39</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>197</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>215</v>
@@ -3056,28 +3045,28 @@
         <v>41</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>197</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>215</v>
@@ -3112,28 +3101,28 @@
         <v>39</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>177</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>213</v>
@@ -3168,28 +3157,28 @@
         <v>41</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>177</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>213</v>
@@ -3224,28 +3213,28 @@
         <v>39</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>193</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>213</v>
@@ -3280,28 +3269,28 @@
         <v>41</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>193</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>213</v>
@@ -3336,28 +3325,28 @@
         <v>39</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>179</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>213</v>
@@ -3392,28 +3381,28 @@
         <v>41</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>179</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>213</v>
@@ -3448,28 +3437,28 @@
         <v>39</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>190</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>215</v>
@@ -3504,28 +3493,28 @@
         <v>41</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>190</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N23" s="4" t="s">
         <v>215</v>
@@ -3560,28 +3549,28 @@
         <v>39</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>194</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>213</v>
@@ -3616,28 +3605,28 @@
         <v>41</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>194</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>213</v>
@@ -3672,28 +3661,28 @@
         <v>39</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>188</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>213</v>
@@ -3728,28 +3717,28 @@
         <v>41</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>188</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>213</v>
@@ -3784,28 +3773,28 @@
         <v>39</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>202</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>213</v>
@@ -3840,28 +3829,28 @@
         <v>41</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>202</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>213</v>
@@ -3896,28 +3885,28 @@
         <v>39</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>183</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>213</v>
@@ -3952,28 +3941,28 @@
         <v>41</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>183</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>213</v>
@@ -4008,28 +3997,28 @@
         <v>39</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>74</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>9</v>
@@ -4064,28 +4053,28 @@
         <v>41</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>73</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>74</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>9</v>
@@ -4120,28 +4109,28 @@
         <v>9</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>78</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>9</v>
@@ -4176,28 +4165,28 @@
         <v>9</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>80</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>81</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>9</v>
@@ -4232,28 +4221,28 @@
         <v>9</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>181</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>9</v>
@@ -4288,28 +4277,28 @@
         <v>88</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>86</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>353</v>
@@ -4344,28 +4333,28 @@
         <v>90</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>86</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>353</v>
@@ -4400,28 +4389,28 @@
         <v>94</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>92</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>203</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>9</v>
@@ -4456,28 +4445,28 @@
         <v>96</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>92</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>203</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>9</v>
@@ -4512,28 +4501,28 @@
         <v>100</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>99</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>221</v>
@@ -4568,28 +4557,28 @@
         <v>102</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="I42" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>99</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>222</v>
@@ -4624,28 +4613,28 @@
         <v>9</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>104</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>211</v>
@@ -4680,28 +4669,28 @@
         <v>108</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>104</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>107</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>211</v>
@@ -4736,28 +4725,28 @@
         <v>19</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>104</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>107</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>211</v>
@@ -4792,28 +4781,28 @@
         <v>21</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>104</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K46" s="4" t="s">
         <v>107</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N46" s="4" t="s">
         <v>211</v>
@@ -4848,28 +4837,28 @@
         <v>9</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>112</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K47" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>211</v>
@@ -4904,28 +4893,28 @@
         <v>9</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>117</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="I48" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K48" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N48" s="4" t="s">
         <v>224</v>
@@ -4960,28 +4949,28 @@
         <v>9</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>117</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K49" s="4" t="s">
         <v>81</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>9</v>
@@ -5016,28 +5005,28 @@
         <v>9</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>117</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="I50" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K50" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>224</v>
@@ -5072,28 +5061,28 @@
         <v>9</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>117</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="I51" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>81</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>9</v>
@@ -5128,28 +5117,28 @@
         <v>94</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>120</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="I52" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K52" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>360</v>
@@ -5184,28 +5173,28 @@
         <v>96</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>120</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="I53" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K53" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>360</v>
@@ -5240,28 +5229,28 @@
         <v>126</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K54" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N54" s="4" t="s">
         <v>360</v>
@@ -5296,28 +5285,28 @@
         <v>128</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I55" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K55" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>360</v>
@@ -5352,28 +5341,28 @@
         <v>130</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I56" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K56" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N56" s="4" t="s">
         <v>360</v>
@@ -5408,28 +5397,28 @@
         <v>132</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>360</v>
@@ -5464,28 +5453,28 @@
         <v>126</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K58" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N58" s="4" t="s">
         <v>360</v>
@@ -5520,28 +5509,28 @@
         <v>128</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I59" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K59" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N59" s="4" t="s">
         <v>360</v>
@@ -5576,28 +5565,28 @@
         <v>130</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I60" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K60" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N60" s="4" t="s">
         <v>360</v>
@@ -5632,28 +5621,28 @@
         <v>132</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K61" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N61" s="4" t="s">
         <v>360</v>
@@ -5688,28 +5677,28 @@
         <v>9</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>138</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="I62" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K62" s="4" t="s">
         <v>176</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N62" s="4" t="s">
         <v>360</v>
@@ -5744,28 +5733,28 @@
         <v>108</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>138</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="I63" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K63" s="4" t="s">
         <v>176</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>360</v>
@@ -5800,28 +5789,28 @@
         <v>19</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>138</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="I64" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K64" s="4" t="s">
         <v>176</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N64" s="4" t="s">
         <v>360</v>
@@ -5856,28 +5845,28 @@
         <v>21</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>138</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K65" s="4" t="s">
         <v>176</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N65" s="4" t="s">
         <v>360</v>
@@ -5912,28 +5901,28 @@
         <v>9</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>144</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="I66" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K66" s="4" t="s">
         <v>8</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N66" s="4" t="s">
         <v>361</v>
@@ -5968,28 +5957,28 @@
         <v>9</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="I67" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K67" s="4" t="s">
         <v>8</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N67" s="4" t="s">
         <v>361</v>
@@ -6024,28 +6013,28 @@
         <v>9</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="I68" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K68" s="4" t="s">
         <v>148</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="M68" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N68" s="4" t="s">
         <v>9</v>
@@ -6080,28 +6069,28 @@
         <v>152</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>150</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="I69" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K69" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N69" s="4" t="s">
         <v>360</v>
@@ -6136,28 +6125,28 @@
         <v>152</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>150</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="I70" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K70" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N70" s="4" t="s">
         <v>360</v>
@@ -6192,28 +6181,28 @@
         <v>157</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>155</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I71" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K71" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N71" s="4" t="s">
         <v>360</v>
@@ -6248,28 +6237,28 @@
         <v>159</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>155</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I72" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K72" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N72" s="4" t="s">
         <v>360</v>
@@ -6304,28 +6293,28 @@
         <v>161</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>155</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I73" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K73" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N73" s="4" t="s">
         <v>360</v>
@@ -6360,28 +6349,28 @@
         <v>163</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>155</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I74" s="4" t="s">
         <v>170</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="K74" s="4" t="s">
         <v>171</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N74" s="4" t="s">
         <v>360</v>
@@ -6416,28 +6405,28 @@
         <v>39</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>165</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="I75" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K75" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N75" s="4" t="s">
         <v>211</v>
@@ -6472,28 +6461,28 @@
         <v>41</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>165</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K76" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N76" s="4" t="s">
         <v>211</v>
@@ -6528,28 +6517,28 @@
         <v>168</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>165</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="I77" s="4" t="s">
         <v>172</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K77" s="4" t="s">
         <v>105</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N77" s="4" t="s">
         <v>211</v>

</xml_diff>

<commit_message>
19Tto20T map - update tb_prev and tx_tb data elements to use coarse ages
</commit_message>
<xml_diff>
--- a/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
+++ b/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/site_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3D6F20AC-ADC3-1E45-B210-BFADB3E73B5C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1DC18066-3BCF-CA49-BCD1-9906104E163E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1750" uniqueCount="438">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1750" uniqueCount="439">
   <si>
     <t>indicatorCode</t>
   </si>
@@ -1347,6 +1347,9 @@
   </si>
   <si>
     <t>2018Oct</t>
+  </si>
+  <si>
+    <t>&lt;15/&gt;15</t>
   </si>
 </sst>
 </file>
@@ -2220,7 +2223,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N61" sqref="E54:N61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5253,7 +5258,7 @@
         <v>437</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="O54" s="4" t="s">
         <v>212</v>
@@ -5309,7 +5314,7 @@
         <v>437</v>
       </c>
       <c r="N55" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="O55" s="4" t="s">
         <v>212</v>
@@ -5365,7 +5370,7 @@
         <v>437</v>
       </c>
       <c r="N56" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="O56" s="4" t="s">
         <v>212</v>
@@ -5421,7 +5426,7 @@
         <v>437</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="O57" s="4" t="s">
         <v>212</v>
@@ -5477,7 +5482,7 @@
         <v>437</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="O58" s="4" t="s">
         <v>212</v>
@@ -5533,7 +5538,7 @@
         <v>437</v>
       </c>
       <c r="N59" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="O59" s="4" t="s">
         <v>212</v>
@@ -5589,7 +5594,7 @@
         <v>437</v>
       </c>
       <c r="N60" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="O60" s="4" t="s">
         <v>212</v>
@@ -5645,7 +5650,7 @@
         <v>437</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="O61" s="4" t="s">
         <v>212</v>
@@ -6205,7 +6210,7 @@
         <v>437</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="O71" s="4" t="s">
         <v>212</v>
@@ -6261,7 +6266,7 @@
         <v>437</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="O72" s="4" t="s">
         <v>212</v>
@@ -6317,7 +6322,7 @@
         <v>437</v>
       </c>
       <c r="N73" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="O73" s="4" t="s">
         <v>212</v>
@@ -6373,7 +6378,7 @@
         <v>437</v>
       </c>
       <c r="N74" s="4" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="O74" s="4" t="s">
         <v>212</v>

</xml_diff>

<commit_message>
19Tto20TMap Changing the disaggregation type of a historic indicator
Related to: https://github.com/pepfar-datim/Global/issues/4577
</commit_message>
<xml_diff>
--- a/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
+++ b/data-raw/site_distribution_configuration/19Tto20TMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/data-pack-commons/data-raw/site_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1DC18066-3BCF-CA49-BCD1-9906104E163E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F564CCAB-0775-9841-9383-62DB622B2F5E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="0" windowWidth="25600" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="19Tto20TMap" sheetId="1" r:id="rId1"/>
@@ -2223,8 +2223,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N61" sqref="E54:N61"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5697,10 +5697,10 @@
         <v>385</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="M62" s="4" t="s">
         <v>437</v>
@@ -6573,9 +6573,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1D6183-4E71-374E-BBB5-F541D22E119E}">
   <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B73" sqref="B73:G76"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>